<commit_message>
H - Added The Customers & Part of The Orders to the Mapping sheets
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Banks" sheetId="9" r:id="rId1"/>
     <sheet name="Withdrawal_All_Accounts_Related" sheetId="8" r:id="rId2"/>
     <sheet name="Withdrawal_Requests" sheetId="5" r:id="rId3"/>
-    <sheet name="Orders" sheetId="1" r:id="rId4"/>
-    <sheet name="Orders_Meta" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
-    <sheet name="Payment_Status_Types_LKP" sheetId="2" r:id="rId7"/>
-    <sheet name="Transactions" sheetId="3" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId9"/>
+    <sheet name="Customers" sheetId="4" r:id="rId4"/>
+    <sheet name="Orders" sheetId="1" r:id="rId5"/>
+    <sheet name="Orders_Meta" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId7"/>
+    <sheet name="Payment_Status_Types_LKP" sheetId="2" r:id="rId8"/>
+    <sheet name="Transactions" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="279">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -704,13 +704,175 @@
   </si>
   <si>
     <t>(1 or 2) as in the Targets's withdrawal types based on some advanced logic from cowpay (withdrawRequests--&gt;1 &amp;Cashout-Transaction[refunds]---&gt;2)</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>`merchant_id`</t>
+  </si>
+  <si>
+    <t>`email`</t>
+  </si>
+  <si>
+    <t>`mobile`</t>
+  </si>
+  <si>
+    <t>`customer_merchant_profile_id`</t>
+  </si>
+  <si>
+    <t>varchar(64)</t>
+  </si>
+  <si>
+    <t>`card_token`</t>
+  </si>
+  <si>
+    <t>varchar(256)</t>
+  </si>
+  <si>
+    <t>`cvv`</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>customers</t>
+  </si>
+  <si>
+    <t>[Email]</t>
+  </si>
+  <si>
+    <t>[MerchantProfileId]</t>
+  </si>
+  <si>
+    <t>[Mobile]</t>
+  </si>
+  <si>
+    <t>Mapping to Customers</t>
+  </si>
+  <si>
+    <t>Fk_Merchant_ID</t>
+  </si>
+  <si>
+    <t>this is the customer's ID at the Merchant System</t>
+  </si>
+  <si>
+    <t>id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">merchant_code </t>
+  </si>
+  <si>
+    <t>promo_code_id</t>
+  </si>
+  <si>
+    <t>payment_gateway </t>
+  </si>
+  <si>
+    <t>channel </t>
+  </si>
+  <si>
+    <t>iframe_id</t>
+  </si>
+  <si>
+    <t>payment_link_type</t>
+  </si>
+  <si>
+    <t>api_access_type</t>
+  </si>
+  <si>
+    <t>payment_method </t>
+  </si>
+  <si>
+    <t>payment_status </t>
+  </si>
+  <si>
+    <t>card_number</t>
+  </si>
+  <si>
+    <t>payment_link_id </t>
+  </si>
+  <si>
+    <t>customer_merchant_profile_id </t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>customer_mobile </t>
+  </si>
+  <si>
+    <t>customer_email</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>card_token</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>init_amount</t>
+  </si>
+  <si>
+    <t>fees_amount</t>
+  </si>
+  <si>
+    <t>vat_amount</t>
+  </si>
+  <si>
+    <t>net_amount</t>
+  </si>
+  <si>
+    <t>currency_code</t>
+  </si>
+  <si>
+    <t>charge_items</t>
+  </si>
+  <si>
+    <t>payment_gateway_reference_id </t>
+  </si>
+  <si>
+    <t>payment_gateway_tracking_number</t>
+  </si>
+  <si>
+    <t>cowpay_commission</t>
+  </si>
+  <si>
+    <t>expires_at</t>
+  </si>
+  <si>
+    <t>paid_at </t>
+  </si>
+  <si>
+    <t>general_extra_data</t>
+  </si>
+  <si>
+    <t>environment</t>
+  </si>
+  <si>
+    <t>`valu_load_number`</t>
+  </si>
+  <si>
+    <t>Mapping to Orders</t>
+  </si>
+  <si>
+    <t>FK_Merchant_Id_Int</t>
+  </si>
+  <si>
+    <t>FK_Merchant_Id_guid</t>
+  </si>
+  <si>
+    <t>currency_code (to be mapped to currency name)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,8 +934,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -828,6 +1003,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -841,14 +1022,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -885,6 +1063,25 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1200,7 +1397,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>214</v>
       </c>
     </row>
@@ -1267,11 +1464,11 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1282,31 +1479,31 @@
       <c r="B1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>151</v>
       </c>
       <c r="N2" t="s">
@@ -1314,39 +1511,39 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N4" t="s">
@@ -1354,28 +1551,28 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>152</v>
       </c>
       <c r="N5" t="s">
@@ -1383,25 +1580,25 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>149</v>
       </c>
       <c r="N6" t="s">
@@ -1409,25 +1606,25 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>149</v>
       </c>
       <c r="N7" t="s">
@@ -1435,28 +1632,28 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>139</v>
       </c>
       <c r="N8" t="s">
@@ -1464,25 +1661,25 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>149</v>
       </c>
       <c r="N9" t="s">
@@ -1490,28 +1687,28 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>141</v>
       </c>
       <c r="N10" t="s">
@@ -1519,28 +1716,28 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
         <v>142</v>
       </c>
       <c r="N11" t="s">
@@ -1548,28 +1745,28 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="11" t="s">
         <v>143</v>
       </c>
       <c r="N12" t="s">
@@ -1577,28 +1774,28 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="11" t="s">
         <v>51</v>
       </c>
       <c r="N13" t="s">
@@ -1606,28 +1803,28 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="11" t="s">
         <v>52</v>
       </c>
       <c r="N14" t="s">
@@ -1635,28 +1832,28 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="11" t="s">
         <v>53</v>
       </c>
       <c r="N15" t="s">
@@ -1664,19 +1861,19 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="11" t="s">
         <v>59</v>
       </c>
       <c r="N16" t="s">
@@ -1684,25 +1881,25 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="11" t="s">
         <v>147</v>
       </c>
       <c r="N17" t="s">
@@ -1710,22 +1907,22 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="K18" s="11" t="s">
         <v>149</v>
       </c>
       <c r="N18" t="s">
@@ -1733,22 +1930,22 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="11">
         <v>1</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="11">
         <v>3</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="11">
         <v>2</v>
       </c>
       <c r="N19" t="s">
@@ -1756,57 +1953,57 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1838,7 +2035,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1866,7 +2063,7 @@
       <c r="C4" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>222</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -1880,13 +2077,13 @@
       <c r="A6" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>162</v>
       </c>
       <c r="C6" t="s">
         <v>174</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>215</v>
       </c>
       <c r="F6" t="s">
@@ -1897,13 +2094,13 @@
       <c r="A7" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>163</v>
       </c>
       <c r="C7" t="s">
         <v>175</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>217</v>
       </c>
       <c r="F7" t="s">
@@ -1917,13 +2114,13 @@
       <c r="A8" t="s">
         <v>172</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>216</v>
       </c>
       <c r="F8" t="s">
@@ -1937,13 +2134,13 @@
       <c r="A9" t="s">
         <v>172</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>165</v>
       </c>
       <c r="C9" t="s">
         <v>176</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="18" t="s">
         <v>163</v>
       </c>
       <c r="F9" t="s">
@@ -1957,13 +2154,13 @@
       <c r="A10" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>166</v>
       </c>
       <c r="C10" t="s">
         <v>177</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="18" t="s">
         <v>219</v>
       </c>
       <c r="F10" t="s">
@@ -1977,13 +2174,13 @@
       <c r="A11" t="s">
         <v>172</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>167</v>
       </c>
       <c r="C11" t="s">
         <v>174</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>220</v>
       </c>
       <c r="F11" t="s">
@@ -1997,13 +2194,13 @@
       <c r="A12" t="s">
         <v>172</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>168</v>
       </c>
       <c r="C12" t="s">
         <v>178</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>224</v>
       </c>
       <c r="F12" t="s">
@@ -2017,13 +2214,13 @@
       <c r="A13" t="s">
         <v>172</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>169</v>
       </c>
       <c r="C13" t="s">
         <v>175</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>223</v>
       </c>
       <c r="F13" t="s">
@@ -2037,13 +2234,13 @@
       <c r="A14" t="s">
         <v>172</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>170</v>
       </c>
       <c r="C14" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="18" t="s">
         <v>167</v>
       </c>
       <c r="F14" t="s">
@@ -2057,13 +2254,13 @@
       <c r="A15" t="s">
         <v>172</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>171</v>
       </c>
       <c r="C15" t="s">
         <v>179</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>168</v>
       </c>
       <c r="F15" t="s">
@@ -2077,13 +2274,13 @@
       <c r="A16" t="s">
         <v>172</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>180</v>
       </c>
       <c r="C16" t="s">
         <v>178</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>180</v>
       </c>
       <c r="F16" t="s">
@@ -2097,13 +2294,13 @@
       <c r="A17" t="s">
         <v>172</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>181</v>
       </c>
       <c r="C17" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="19" t="s">
         <v>181</v>
       </c>
       <c r="F17" t="s">
@@ -2114,7 +2311,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>182</v>
       </c>
       <c r="F18" t="s">
@@ -2125,7 +2322,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>182</v>
       </c>
       <c r="F19" t="s">
@@ -2148,244 +2345,222 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="B2:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="89.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E5" t="s">
+    <row r="2" spans="2:13" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="B2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="J4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E21" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
+    </row>
+    <row r="5" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="J6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="J7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
+        <v>193</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="J8" t="s">
+        <v>237</v>
+      </c>
+      <c r="M8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="J9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" t="s">
+        <v>232</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="J10" t="s">
         <v>51</v>
       </c>
-      <c r="F25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E26" t="s">
+    </row>
+    <row r="11" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="J11" t="s">
         <v>52</v>
       </c>
-      <c r="F26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E27" t="s">
+    </row>
+    <row r="12" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" t="s">
+        <v>178</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J12" t="s">
         <v>53</v>
       </c>
-      <c r="F27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E28" t="s">
-        <v>54</v>
-      </c>
-      <c r="F28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E30" t="s">
-        <v>0</v>
+    </row>
+    <row r="13" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" t="s">
+        <v>178</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2395,6 +2570,432 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="51.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B6" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B7" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="D7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" t="s">
+        <v>277</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B12" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B13" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B16" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B17" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B18" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B19" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B20" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B21" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B22" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="F23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B24" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="F24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B25" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B26" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="F26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B27" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B28" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B29" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B30" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="F30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B31" s="29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B32" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B33" s="26" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B34" s="26" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B35" s="26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B36" s="26" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B37" s="26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B38" s="28" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B39" s="26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>274</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -2571,7 +3172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2585,7 +3186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2599,11 +3200,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2796,16 +3397,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
More Progress in the Mapping Sheets . Orders
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="300">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -859,13 +859,76 @@
     <t>Mapping to Orders</t>
   </si>
   <si>
-    <t>FK_Merchant_Id_Int</t>
-  </si>
-  <si>
-    <t>FK_Merchant_Id_guid</t>
-  </si>
-  <si>
     <t>currency_code (to be mapped to currency name)</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>customer_id(Needs to be mapped on the customers Table IDs)</t>
+  </si>
+  <si>
+    <t>Calculated using some Logic</t>
+  </si>
+  <si>
+    <t>Calculated Column</t>
+  </si>
+  <si>
+    <t>Auto Generated</t>
+  </si>
+  <si>
+    <t>one to one</t>
+  </si>
+  <si>
+    <t>Brought from another Table</t>
+  </si>
+  <si>
+    <t>[ChannelTypeId]</t>
+  </si>
+  <si>
+    <t>[PaymentLinkId]</t>
+  </si>
+  <si>
+    <t>[PaymentMethodTypeId]</t>
+  </si>
+  <si>
+    <t>[CardNumber]</t>
+  </si>
+  <si>
+    <t>[Token]</t>
+  </si>
+  <si>
+    <t>[ExtraData]</t>
+  </si>
+  <si>
+    <t>[PGWMetaRequest]</t>
+  </si>
+  <si>
+    <t>[PromoCode]</t>
+  </si>
+  <si>
+    <t>[ReturnURL]</t>
+  </si>
+  <si>
+    <t>[OrderMeta]</t>
+  </si>
+  <si>
+    <t>[Orders]</t>
+  </si>
+  <si>
+    <t>FK_Merchant_Id_Int (needs Mapping on Merchants)</t>
+  </si>
+  <si>
+    <t>FK_Merchant_Id_guid (needs Mapping on Merchants)</t>
+  </si>
+  <si>
+    <t>(fk_of Currency) (needs Mapping on Currency )</t>
+  </si>
+  <si>
+    <t>payment_gateway_reference_id (Needs to be Mapped on PGW id)</t>
+  </si>
+  <si>
+    <t>api_access_type (Needs Mapping on Access Types id)</t>
   </si>
 </sst>
 </file>
@@ -948,7 +1011,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1009,6 +1072,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1022,7 +1103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1064,9 +1145,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1081,6 +1159,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1455,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C16" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1479,16 +1568,16 @@
       <c r="B1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E2" s="13" t="s">
@@ -2035,7 +2124,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2383,7 +2472,7 @@
       <c r="B4" t="s">
         <v>235</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>187</v>
       </c>
       <c r="D4" t="s">
@@ -2400,13 +2489,13 @@
       <c r="B5" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>226</v>
       </c>
       <c r="D5" t="s">
         <v>174</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>240</v>
       </c>
       <c r="J5" t="s">
@@ -2417,13 +2506,13 @@
       <c r="B6" t="s">
         <v>235</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>227</v>
       </c>
       <c r="D6" t="s">
         <v>193</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="24" t="s">
         <v>196</v>
       </c>
       <c r="J6" t="s">
@@ -2434,13 +2523,13 @@
       <c r="B7" t="s">
         <v>235</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>228</v>
       </c>
       <c r="D7" t="s">
         <v>193</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>227</v>
       </c>
       <c r="J7" t="s">
@@ -2451,13 +2540,13 @@
       <c r="B8" t="s">
         <v>235</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>196</v>
       </c>
       <c r="D8" t="s">
         <v>193</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="22" t="s">
         <v>229</v>
       </c>
       <c r="J8" t="s">
@@ -2471,13 +2560,13 @@
       <c r="B9" t="s">
         <v>235</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>229</v>
       </c>
       <c r="D9" t="s">
         <v>230</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="24" t="s">
         <v>228</v>
       </c>
       <c r="J9" t="s">
@@ -2488,13 +2577,13 @@
       <c r="B10" t="s">
         <v>235</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>231</v>
       </c>
       <c r="D10" t="s">
         <v>232</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="24" t="s">
         <v>199</v>
       </c>
       <c r="J10" t="s">
@@ -2505,13 +2594,13 @@
       <c r="B11" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>233</v>
       </c>
       <c r="D11" t="s">
         <v>174</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="24" t="s">
         <v>200</v>
       </c>
       <c r="J11" t="s">
@@ -2522,13 +2611,13 @@
       <c r="B12" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="21" t="s">
         <v>199</v>
       </c>
       <c r="D12" t="s">
         <v>178</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>201</v>
       </c>
       <c r="J12" t="s">
@@ -2539,13 +2628,13 @@
       <c r="B13" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="21" t="s">
         <v>200</v>
       </c>
       <c r="D13" t="s">
         <v>178</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="24" t="s">
         <v>182</v>
       </c>
       <c r="J13" t="s">
@@ -2556,7 +2645,7 @@
       <c r="B14" t="s">
         <v>235</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="21" t="s">
         <v>201</v>
       </c>
       <c r="D14" t="s">
@@ -2571,16 +2660,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="42.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2612,12 +2701,15 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>242</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>215</v>
       </c>
+      <c r="E5" t="s">
+        <v>294</v>
+      </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
@@ -2626,8 +2718,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>243</v>
+      </c>
+      <c r="E6" t="s">
+        <v>294</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -2637,11 +2732,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="D7" t="s">
-        <v>276</v>
+      <c r="D7" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="E7" t="s">
+        <v>294</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -2651,11 +2749,14 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="D8" t="s">
-        <v>277</v>
+      <c r="D8" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="E8" t="s">
+        <v>294</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -2665,8 +2766,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>246</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="E9" t="s">
+        <v>294</v>
       </c>
       <c r="F9" t="s">
         <v>19</v>
@@ -2676,8 +2783,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>247</v>
+      </c>
+      <c r="E10" t="s">
+        <v>294</v>
       </c>
       <c r="F10" t="s">
         <v>21</v>
@@ -2687,11 +2797,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="28" t="s">
         <v>254</v>
+      </c>
+      <c r="E11" t="s">
+        <v>294</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
@@ -2701,8 +2814,14 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="33" t="s">
         <v>249</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" t="s">
+        <v>294</v>
       </c>
       <c r="F12" t="s">
         <v>25</v>
@@ -2712,8 +2831,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>250</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" t="s">
+        <v>294</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
@@ -2723,8 +2848,14 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>251</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="E14" t="s">
+        <v>294</v>
       </c>
       <c r="F14" t="s">
         <v>29</v>
@@ -2734,8 +2865,14 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>252</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="E15" t="s">
+        <v>294</v>
       </c>
       <c r="F15" t="s">
         <v>31</v>
@@ -2745,8 +2882,14 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>253</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="E16" t="s">
+        <v>294</v>
       </c>
       <c r="F16" t="s">
         <v>33</v>
@@ -2756,8 +2899,14 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>254</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" t="s">
+        <v>294</v>
       </c>
       <c r="F17" t="s">
         <v>35</v>
@@ -2767,11 +2916,14 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>255</v>
       </c>
-      <c r="D18" t="s">
-        <v>38</v>
+      <c r="D18" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="E18" t="s">
+        <v>294</v>
       </c>
       <c r="F18" t="s">
         <v>37</v>
@@ -2781,11 +2933,14 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>256</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>278</v>
+      <c r="D19" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="E19" t="s">
+        <v>294</v>
       </c>
       <c r="F19" t="s">
         <v>39</v>
@@ -2795,11 +2950,14 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>166</v>
+      </c>
+      <c r="E20" t="s">
+        <v>294</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
@@ -2809,8 +2967,11 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>258</v>
+      </c>
+      <c r="E21" t="s">
+        <v>294</v>
       </c>
       <c r="F21" t="s">
         <v>43</v>
@@ -2820,8 +2981,14 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>169</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="E22" t="s">
+        <v>294</v>
       </c>
       <c r="F22" t="s">
         <v>45</v>
@@ -2831,8 +2998,11 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>259</v>
+      </c>
+      <c r="E23" t="s">
+        <v>294</v>
       </c>
       <c r="F23" t="s">
         <v>47</v>
@@ -2842,8 +3012,11 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="25" t="s">
         <v>260</v>
+      </c>
+      <c r="E24" t="s">
+        <v>294</v>
       </c>
       <c r="F24" t="s">
         <v>49</v>
@@ -2853,11 +3026,14 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="23" t="s">
         <v>199</v>
+      </c>
+      <c r="E25" t="s">
+        <v>294</v>
       </c>
       <c r="F25" t="s">
         <v>51</v>
@@ -2867,11 +3043,14 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="23" t="s">
         <v>200</v>
+      </c>
+      <c r="E26" t="s">
+        <v>294</v>
       </c>
       <c r="F26" t="s">
         <v>52</v>
@@ -2881,11 +3060,14 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="23" t="s">
         <v>201</v>
+      </c>
+      <c r="E27" t="s">
+        <v>294</v>
       </c>
       <c r="F27" t="s">
         <v>53</v>
@@ -2895,8 +3077,11 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>263</v>
+      </c>
+      <c r="E28" t="s">
+        <v>294</v>
       </c>
       <c r="F28" t="s">
         <v>54</v>
@@ -2906,8 +3091,11 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="25" t="s">
         <v>264</v>
+      </c>
+      <c r="E29" t="s">
+        <v>294</v>
       </c>
       <c r="F29" t="s">
         <v>55</v>
@@ -2917,7 +3105,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>265</v>
       </c>
       <c r="F30" t="s">
@@ -2925,68 +3113,267 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="25" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B33" s="26" t="s">
+      <c r="E32" t="s">
+        <v>293</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B33" s="33" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B34" s="26" t="s">
+      <c r="D33" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="E33" t="s">
+        <v>293</v>
+      </c>
+      <c r="F33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B34" s="25" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B35" s="26" t="s">
+      <c r="D34" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="E34" t="s">
+        <v>293</v>
+      </c>
+      <c r="F34" t="s">
+        <v>284</v>
+      </c>
+      <c r="G34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B35" s="25" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B36" s="26" t="s">
+      <c r="E35" t="s">
+        <v>293</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B36" s="25" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B37" s="26" t="s">
+      <c r="E36" t="s">
+        <v>293</v>
+      </c>
+      <c r="F36" t="s">
+        <v>285</v>
+      </c>
+      <c r="G36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B37" s="28" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B38" s="28" t="s">
+      <c r="E37" t="s">
+        <v>293</v>
+      </c>
+      <c r="F37" t="s">
+        <v>286</v>
+      </c>
+      <c r="G37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B38" s="27" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="39" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B39" s="26" t="s">
+      <c r="E38" t="s">
+        <v>293</v>
+      </c>
+      <c r="F38" t="s">
+        <v>287</v>
+      </c>
+      <c r="G38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B39" s="25" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" s="24" t="s">
+      <c r="E39" t="s">
+        <v>293</v>
+      </c>
+      <c r="F39" t="s">
+        <v>288</v>
+      </c>
+      <c r="G39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="23" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" s="24" t="s">
+      <c r="E40" t="s">
+        <v>293</v>
+      </c>
+      <c r="F40" t="s">
+        <v>289</v>
+      </c>
+      <c r="G40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="23" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B42" s="24" t="s">
+      <c r="E41" t="s">
+        <v>293</v>
+      </c>
+      <c r="F41" t="s">
+        <v>290</v>
+      </c>
+      <c r="G41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="23" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>293</v>
+      </c>
+      <c r="F42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>274</v>
+      </c>
+      <c r="E43" t="s">
+        <v>293</v>
+      </c>
+      <c r="F43" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
+        <v>293</v>
+      </c>
+      <c r="F44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E45" t="s">
+        <v>293</v>
+      </c>
+      <c r="F45" t="s">
+        <v>292</v>
+      </c>
+      <c r="G45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E46" t="s">
+        <v>293</v>
+      </c>
+      <c r="F46" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E47" t="s">
+        <v>293</v>
+      </c>
+      <c r="F47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>293</v>
+      </c>
+      <c r="F48" t="s">
+        <v>53</v>
+      </c>
+      <c r="G48" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E49" t="s">
+        <v>293</v>
+      </c>
+      <c r="F49" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B57" s="30" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B58" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="23" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="32" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3000,7 +3387,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F6" sqref="F6:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
m & H modified the Merchansts task and The Mapping sheets
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="429">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1312,71 +1312,17 @@
     <t>WithdrawalRequestTransactions TRGT Columns</t>
   </si>
   <si>
-    <t>added_to_merchant_available_balance</t>
-  </si>
-  <si>
-    <t>merchant_net_amount</t>
-  </si>
-  <si>
-    <t>merchant_code</t>
-  </si>
-  <si>
-    <t>transaction_number</t>
-  </si>
-  <si>
-    <t>transaction_date</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Transactions SRC</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>int_amount</t>
-  </si>
-  <si>
-    <t>accountant_id</t>
-  </si>
-  <si>
-    <t>model_id</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>deleted_at</t>
-  </si>
-  <si>
-    <t>w_id</t>
-  </si>
-  <si>
-    <t>merchant_id</t>
-  </si>
-  <si>
-    <t>w_amount</t>
-  </si>
-  <si>
-    <t>w_description</t>
-  </si>
-  <si>
-    <t>w_created_at</t>
-  </si>
-  <si>
-    <t>w_updated_at</t>
-  </si>
-  <si>
-    <t>merchant_reference_id</t>
+    <t>SELECT a.* FROM cowpay_staging.transactions a join withdrawal_requests b on a.transaction_number=b.id;</t>
+  </si>
+  <si>
+    <t>Src_Table Transactions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1522,14 +1468,8 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1614,12 +1554,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDFDFE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1633,7 +1567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1755,14 +1689,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2051,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -2746,7 +2674,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3324,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3333,7 +3261,8 @@
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.21875" customWidth="1"/>
-    <col min="4" max="4" width="74.88671875" customWidth="1"/>
+    <col min="4" max="4" width="172.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" customWidth="1"/>
     <col min="6" max="6" width="78.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -3635,310 +3564,194 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P34"/>
+  <dimension ref="A2:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="54.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="61.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="81" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.44140625" customWidth="1"/>
+    <col min="3" max="5" width="6.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="81" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" t="s">
         <v>222</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="J2" t="s">
-        <v>222</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D4" s="55" t="s">
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="55" t="s">
         <v>427</v>
       </c>
-      <c r="K4" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="L4" t="s">
+      <c r="H4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D5" s="56" t="s">
-        <v>435</v>
-      </c>
-      <c r="K5" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
         <v>417</v>
       </c>
-      <c r="L5" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D6" s="56" t="s">
-        <v>152</v>
-      </c>
-      <c r="K6" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
         <v>418</v>
       </c>
-      <c r="L6" t="s">
+      <c r="H6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D7" s="56" t="s">
-        <v>250</v>
-      </c>
-      <c r="K7" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
         <v>105</v>
       </c>
-      <c r="L7" t="s">
+      <c r="H7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D8" s="56" t="s">
-        <v>251</v>
-      </c>
-      <c r="K8" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
         <v>84</v>
       </c>
-      <c r="L8" t="s">
+      <c r="H8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D9" s="56" t="s">
-        <v>428</v>
-      </c>
-      <c r="K9" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
         <v>419</v>
       </c>
-      <c r="L9" t="s">
+      <c r="H9" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D10" s="55" t="s">
-        <v>429</v>
-      </c>
-      <c r="K10" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
         <v>420</v>
       </c>
-      <c r="L10" t="s">
+      <c r="H10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D11" s="56" t="s">
-        <v>436</v>
-      </c>
-      <c r="K11" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="L11" t="s">
+      <c r="H11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D12" s="56" t="s">
-        <v>430</v>
-      </c>
-      <c r="K12" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
         <v>30</v>
       </c>
-      <c r="L12" t="s">
+      <c r="H12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D13" s="56" t="s">
-        <v>431</v>
-      </c>
-      <c r="K13" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
         <v>421</v>
       </c>
-      <c r="L13" t="s">
+      <c r="H13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D14" s="56" t="s">
-        <v>437</v>
-      </c>
-      <c r="K14" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
         <v>94</v>
       </c>
-      <c r="L14" t="s">
+      <c r="H14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D15" s="57" t="s">
-        <v>438</v>
-      </c>
-      <c r="K15" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
         <v>96</v>
       </c>
-      <c r="L15" t="s">
+      <c r="H15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D16" s="56" t="s">
-        <v>155</v>
-      </c>
-      <c r="K16" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
         <v>422</v>
       </c>
-      <c r="L16" t="s">
+      <c r="H16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="4:12" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="D17" s="56" t="s">
-        <v>432</v>
-      </c>
-      <c r="K17" t="s">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
         <v>423</v>
       </c>
-      <c r="L17" t="s">
+      <c r="H17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>261</v>
-      </c>
-      <c r="K18" t="s">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
         <v>424</v>
       </c>
-      <c r="L18" t="s">
+      <c r="H18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
-        <v>169</v>
-      </c>
-      <c r="K19" t="s">
+    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
         <v>50</v>
       </c>
-      <c r="L19" t="s">
+      <c r="H19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
-        <v>170</v>
-      </c>
-      <c r="K20" t="s">
+    <row r="20" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
         <v>51</v>
       </c>
-      <c r="L20" t="s">
+      <c r="H20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>439</v>
-      </c>
-      <c r="K21" t="s">
+    <row r="21" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
         <v>52</v>
       </c>
-      <c r="L21" t="s">
+      <c r="H21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>440</v>
-      </c>
-      <c r="K22" t="s">
+    <row r="22" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
         <v>57</v>
       </c>
-      <c r="L22" t="s">
+      <c r="H22" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D31" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D34" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4177,8 +3990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
h-Slight Modification in Transactions Mapping Sheet
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="455">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1659,7 +1659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1788,6 +1788,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2076,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2730,12 +2733,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -2785,8 +2788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3362,10 +3365,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3431,7 +3434,7 @@
       <c r="C7" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="59" t="s">
         <v>204</v>
       </c>
       <c r="F7" t="s">
@@ -3451,7 +3454,7 @@
       <c r="C8" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="59" t="s">
         <v>203</v>
       </c>
       <c r="F8" t="s">
@@ -3672,6 +3675,31 @@
       </c>
       <c r="F20" s="51" t="s">
         <v>446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="22" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="30" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -4256,7 +4284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B57" sqref="B57:B61"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
H- Added Some Modifications to The Mapping Sheet & Implemented The Mobile Wallets Tables Maps
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="487">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1397,9 +1397,6 @@
     <t>SELECT distinct status FROM cowpay_staging.withdrawal_requests;</t>
   </si>
   <si>
-    <t>CardMetaData</t>
-  </si>
-  <si>
     <t>8-Src Table of PaymentLinkType</t>
   </si>
   <si>
@@ -1464,13 +1461,43 @@
   </si>
   <si>
     <t>char</t>
+  </si>
+  <si>
+    <t>fk_Customers</t>
+  </si>
+  <si>
+    <t>convert(char(6),first_six)+'******'+convert(char(4),last_four)</t>
+  </si>
+  <si>
+    <t>MerchantId</t>
+  </si>
+  <si>
+    <t>old_fk_Customer_Id</t>
+  </si>
+  <si>
+    <t>auto_Generated</t>
+  </si>
+  <si>
+    <t>old_Customer_Id</t>
+  </si>
+  <si>
+    <t>old_bank_id</t>
+  </si>
+  <si>
+    <t>old_wallet_ID</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Conditional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1624,8 +1651,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1716,6 +1751,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1738,7 +1779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1856,6 +1897,7 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1871,7 +1913,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2157,10 +2205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F66"/>
+  <dimension ref="A2:H66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2172,7 +2220,7 @@
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
         <v>391</v>
       </c>
@@ -2188,7 +2236,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>188</v>
       </c>
@@ -2198,7 +2246,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2210,7 +2258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="15" t="s">
         <v>187</v>
@@ -2224,7 +2272,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="15" t="s">
         <v>155</v>
@@ -2238,7 +2286,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="15" t="s">
         <v>156</v>
@@ -2252,7 +2300,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="15"/>
       <c r="C8" s="10"/>
@@ -2264,7 +2312,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="15"/>
       <c r="C9" s="10"/>
@@ -2276,7 +2324,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="32" t="s">
         <v>392</v>
       </c>
@@ -2291,8 +2340,11 @@
       <c r="F11" s="32" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="H11" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>274</v>
       </c>
@@ -2302,7 +2354,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="15"/>
       <c r="C13" s="10"/>
@@ -2314,7 +2366,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="15" t="s">
         <v>273</v>
@@ -2328,7 +2380,8 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="32" t="s">
         <v>393</v>
       </c>
@@ -2380,6 +2433,7 @@
         <v>273</v>
       </c>
     </row>
+    <row r="20" spans="1:6" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="32" t="s">
         <v>394</v>
@@ -2480,6 +2534,7 @@
         <v>55</v>
       </c>
     </row>
+    <row r="29" spans="1:6" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="32" t="s">
         <v>395</v>
@@ -2518,7 +2573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>286</v>
@@ -2532,7 +2587,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -2544,7 +2599,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2556,7 +2611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -2568,7 +2623,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -2580,7 +2635,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -2592,7 +2647,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="32" t="s">
         <v>396</v>
       </c>
@@ -2607,8 +2663,11 @@
       <c r="F40" s="32" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H40" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>296</v>
       </c>
@@ -2618,7 +2677,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -2630,7 +2689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
         <v>297</v>
@@ -2644,7 +2703,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -2656,7 +2715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -2668,7 +2727,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -2680,7 +2739,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2692,7 +2751,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2704,7 +2763,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A50" s="32" t="s">
         <v>452</v>
       </c>
@@ -2719,8 +2779,11 @@
       <c r="F50" s="32" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H50" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>454</v>
       </c>
@@ -2730,7 +2793,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -2742,7 +2805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
         <v>141</v>
@@ -2756,7 +2819,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -2768,7 +2831,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -2778,7 +2841,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -2788,7 +2851,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -2798,14 +2861,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F58" t="s">
+    <row r="58" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="61" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A59" s="32" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B59" s="32" t="s">
         <v>186</v>
@@ -2819,7 +2882,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>303</v>
       </c>
@@ -2829,7 +2892,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -2841,7 +2904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="10"/>
       <c r="B62" s="10" t="s">
         <v>221</v>
@@ -2855,7 +2918,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -2867,7 +2930,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -2921,30 +2984,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="57" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="J1" s="57" t="s">
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="J1" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="O1" s="58" t="s">
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="O1" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="T1" s="59" t="s">
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="T1" s="60" t="s">
         <v>314</v>
       </c>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="60"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
@@ -3655,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3691,11 +3754,6 @@
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>455</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3705,8 +3763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3729,16 +3787,16 @@
       <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F2" s="13" t="s">
@@ -3811,7 +3869,7 @@
         <v>163</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>113</v>
@@ -3820,7 +3878,7 @@
         <v>121</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>128</v>
@@ -4014,7 +4072,7 @@
         <v>119</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>157</v>
+        <v>486</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>119</v>
@@ -4211,6 +4269,15 @@
       </c>
       <c r="C20" s="10" t="s">
         <v>168</v>
+      </c>
+      <c r="G20" s="63" t="s">
+        <v>483</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="K20" s="63" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -4277,6 +4344,7 @@
     <mergeCell ref="G1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4285,7 +4353,7 @@
   <dimension ref="B2:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4327,8 +4395,8 @@
       <c r="D4" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="20" t="s">
-        <v>162</v>
+      <c r="H4" s="62" t="s">
+        <v>481</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
@@ -4499,6 +4567,12 @@
       </c>
       <c r="D14" t="s">
         <v>153</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -4509,10 +4583,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J19"/>
+  <dimension ref="A3:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4520,7 +4594,7 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.44140625" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -4552,7 +4626,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B4" t="s">
         <v>409</v>
@@ -4568,104 +4642,134 @@
       <c r="C5" t="s">
         <v>150</v>
       </c>
+      <c r="E5" t="s">
+        <v>437</v>
+      </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
       </c>
+      <c r="E6" t="s">
+        <v>477</v>
+      </c>
       <c r="G6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C7" t="s">
         <v>150</v>
       </c>
+      <c r="E7" s="28" t="s">
+        <v>478</v>
+      </c>
       <c r="G7" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C8" t="s">
         <v>163</v>
       </c>
+      <c r="E8" s="52" t="s">
+        <v>467</v>
+      </c>
       <c r="G8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="B9" s="52" t="s">
         <v>233</v>
       </c>
       <c r="C9" t="s">
         <v>150</v>
       </c>
+      <c r="E9" s="52" t="s">
+        <v>468</v>
+      </c>
       <c r="G9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>468</v>
+      <c r="B10" s="52" t="s">
+        <v>467</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
       </c>
+      <c r="E10" s="52" t="s">
+        <v>471</v>
+      </c>
       <c r="G10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>469</v>
+      <c r="B11" s="52" t="s">
+        <v>468</v>
       </c>
       <c r="C11" t="s">
         <v>150</v>
       </c>
+      <c r="E11" s="52" t="s">
+        <v>470</v>
+      </c>
       <c r="G11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
       </c>
+      <c r="E12" s="52" t="s">
+        <v>233</v>
+      </c>
       <c r="G12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="52" t="s">
+        <v>470</v>
+      </c>
+      <c r="C13" t="s">
+        <v>476</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="G13" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="52" t="s">
         <v>471</v>
       </c>
-      <c r="C13" t="s">
-        <v>477</v>
-      </c>
-      <c r="G13" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>472</v>
-      </c>
       <c r="C14" t="s">
-        <v>477</v>
+        <v>476</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>155</v>
       </c>
       <c r="G14" t="s">
         <v>48</v>
@@ -4673,54 +4777,104 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>472</v>
+      </c>
+      <c r="C15" t="s">
         <v>473</v>
       </c>
-      <c r="C15" t="s">
-        <v>474</v>
+      <c r="E15" s="52" t="s">
+        <v>156</v>
       </c>
       <c r="G15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="B16" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="C16" t="s">
         <v>475</v>
       </c>
-      <c r="C16" t="s">
-        <v>476</v>
+      <c r="E16" s="52" t="s">
+        <v>419</v>
       </c>
       <c r="G16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="B17" s="52" t="s">
         <v>155</v>
       </c>
       <c r="C17" t="s">
         <v>153</v>
       </c>
+      <c r="E17" t="s">
+        <v>157</v>
+      </c>
       <c r="G17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="B18" s="52" t="s">
         <v>156</v>
       </c>
       <c r="C18" t="s">
         <v>153</v>
       </c>
-      <c r="G18" t="s">
-        <v>92</v>
+      <c r="E18" t="s">
+        <v>464</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+      <c r="B19" s="52" t="s">
         <v>419</v>
       </c>
       <c r="C19" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G20" s="61" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>413</v>
+      </c>
+      <c r="G21" s="61" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C22" s="28" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C23" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C24" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C25" s="22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C26" s="30" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -4733,7 +4887,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5007,7 +5161,7 @@
       <c r="D20" s="51" t="s">
         <v>409</v>
       </c>
-      <c r="F20" s="51" t="s">
+      <c r="F20" s="64" t="s">
         <v>426</v>
       </c>
     </row>
@@ -5046,8 +5200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5353,7 +5507,7 @@
       <c r="D23" s="22" t="s">
         <v>416</v>
       </c>
-      <c r="G23" s="52" t="s">
+      <c r="G23" s="65" t="s">
         <v>446</v>
       </c>
     </row>
@@ -5393,7 +5547,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6291,7 +6445,7 @@
       <c r="D50" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="9" t="s">
         <v>444</v>
       </c>
     </row>
@@ -6331,7 +6485,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6507,7 +6661,7 @@
       <c r="B16" s="22" t="s">
         <v>424</v>
       </c>
-      <c r="D16" s="60"/>
+      <c r="D16" s="55"/>
       <c r="F16" t="s">
         <v>402</v>
       </c>
@@ -6519,7 +6673,7 @@
       <c r="B17" t="s">
         <v>415</v>
       </c>
-      <c r="D17" s="60"/>
+      <c r="D17" s="55"/>
       <c r="F17" t="s">
         <v>84</v>
       </c>
@@ -6683,7 +6837,7 @@
       <c r="D31" t="s">
         <v>416</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="9" t="s">
         <v>445</v>
       </c>
     </row>

</xml_diff>

<commit_message>
H- Added Some Important Cleansing Activities to Mearchants
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="487">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1898,6 +1898,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1913,13 +1920,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2324,7 +2324,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="32" t="s">
         <v>392</v>
@@ -2380,7 +2380,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="32" t="s">
         <v>393</v>
@@ -2433,7 +2433,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="32" t="s">
         <v>394</v>
@@ -2534,7 +2534,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="32" t="s">
         <v>395</v>
@@ -2647,7 +2647,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="32" t="s">
         <v>396</v>
@@ -2763,7 +2763,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A50" s="32" t="s">
         <v>452</v>
@@ -2861,8 +2861,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F58" s="61" t="s">
+    <row r="58" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="56" t="s">
         <v>304</v>
       </c>
     </row>
@@ -2984,30 +2984,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="62" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="J1" s="58" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="J1" s="63" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="O1" s="59" t="s">
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="O1" s="64" t="s">
         <v>313</v>
       </c>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="T1" s="60" t="s">
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="T1" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
@@ -3763,8 +3763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3787,16 +3787,16 @@
       <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F2" s="13" t="s">
@@ -4205,7 +4205,7 @@
         <v>123</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="K17" s="11" t="s">
         <v>123</v>
@@ -4270,13 +4270,13 @@
       <c r="C20" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="58" t="s">
         <v>483</v>
       </c>
       <c r="J20" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="K20" s="63" t="s">
+      <c r="K20" s="58" t="s">
         <v>484</v>
       </c>
     </row>
@@ -4350,10 +4350,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M14"/>
+  <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4395,7 +4395,7 @@
       <c r="D4" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="62" t="s">
+      <c r="H4" s="57" t="s">
         <v>481</v>
       </c>
       <c r="J4" t="s">
@@ -4573,6 +4573,31 @@
       </c>
       <c r="J14" s="9" t="s">
         <v>482</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="28" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="22" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="30" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -4585,15 +4610,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.44140625" customWidth="1"/>
@@ -4840,7 +4865,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="61" t="s">
+      <c r="G20" s="56" t="s">
         <v>479</v>
       </c>
     </row>
@@ -4848,7 +4873,7 @@
       <c r="E21" t="s">
         <v>413</v>
       </c>
-      <c r="G21" s="61" t="s">
+      <c r="G21" s="56" t="s">
         <v>413</v>
       </c>
     </row>
@@ -5161,7 +5186,7 @@
       <c r="D20" s="51" t="s">
         <v>409</v>
       </c>
-      <c r="F20" s="64" t="s">
+      <c r="F20" s="59" t="s">
         <v>426</v>
       </c>
     </row>
@@ -5507,7 +5532,7 @@
       <c r="D23" s="22" t="s">
         <v>416</v>
       </c>
-      <c r="G23" s="65" t="s">
+      <c r="G23" s="60" t="s">
         <v>446</v>
       </c>
     </row>

</xml_diff>

<commit_message>
H- Added The Bank Accounts and The All Accounts to the Transaction Management & the Neat trick to keep going
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="488">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1491,6 +1491,9 @@
   </si>
   <si>
     <t>Conditional</t>
+  </si>
+  <si>
+    <t>old_fawry_id</t>
   </si>
 </sst>
 </file>
@@ -2207,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3763,8 +3766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4273,11 +4276,17 @@
       <c r="G20" s="58" t="s">
         <v>483</v>
       </c>
+      <c r="I20" s="58" t="s">
+        <v>487</v>
+      </c>
       <c r="J20" s="12" t="s">
         <v>409</v>
       </c>
       <c r="K20" s="58" t="s">
         <v>484</v>
+      </c>
+      <c r="N20" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -4353,7 +4362,7 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4610,8 +4619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4912,7 +4921,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4923,7 +4932,7 @@
     <col min="4" max="4" width="172.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.109375" customWidth="1"/>
     <col min="6" max="6" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5225,8 +5234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added to the Transactions mapping sheet, in the withdrawalrequests the model types that we won't be Migrating like orders, topups,blocked amount
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="495">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1494,6 +1494,27 @@
   </si>
   <si>
     <t>old_fawry_id</t>
+  </si>
+  <si>
+    <t>what we won't be migrating is simply all the Withdraw requests whith model types</t>
+  </si>
+  <si>
+    <t>App\Models\WithdrawalRequest</t>
+  </si>
+  <si>
+    <t>App\Models\BlockedAmount</t>
+  </si>
+  <si>
+    <t>App\Models\Order</t>
+  </si>
+  <si>
+    <t>App\Models\Cashout</t>
+  </si>
+  <si>
+    <t>App\Modules\Order\Models\Order</t>
+  </si>
+  <si>
+    <t>App\Models\Topup</t>
   </si>
 </sst>
 </file>
@@ -3766,7 +3787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
@@ -4362,7 +4383,7 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4918,10 +4939,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5222,6 +5243,41 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="30" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D30" s="56" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="56" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H- Added Notes to what's Left to be done later in the Transaction Mapping Sheet
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="503">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1515,6 +1515,46 @@
   </si>
   <si>
     <t>App\Models\Topup</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Bank Accounts Needs to be revisited when The Banks LKPs Is Finished (connect The Bank Accounts PRepared To the LKP_DB.Banks_Src )</t>
+  </si>
+  <si>
+    <t>The Handeled By Column needs to be revisited when idenitiy_DB is Migrated (Add the FK from The Users Table)</t>
+  </si>
+  <si>
+    <t>SELECT
+co.*
+,t.[model_id]
+,t.[model]
+,t.[type]
+  FROM cashouts co 
+  left join  
+  (select * from transactions 
+  where model='App\Models\WithdrawalRequest') as t on t.model_id=co.id</t>
+  </si>
+  <si>
+    <t>Union All</t>
+  </si>
+  <si>
+    <t>SELECT
+wr.*
+,t.[model_id]
+,t.[model]
+,t.[type]
+  FROM withdrawal_requests wr 
+  left join  
+  (select * from transactions 
+  where model='App\Models\WithdrawalRequest') as t on t.model_id=wr.id</t>
+  </si>
+  <si>
+    <t>Columns : [CustomerAmount], [MerchantAmount] Needs to be revisited by meeting with Zain &amp; khalaf</t>
   </si>
 </sst>
 </file>
@@ -1803,7 +1843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1943,6 +1983,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2231,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3745,7 +3788,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4321,7 +4364,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>183</v>
       </c>
@@ -4330,6 +4373,9 @@
       </c>
       <c r="C22" s="10" t="s">
         <v>153</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -4341,6 +4387,9 @@
       </c>
       <c r="C23" s="10" t="s">
         <v>153</v>
+      </c>
+      <c r="M23" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -4382,8 +4431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4641,7 +4690,7 @@
   <dimension ref="A3:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4939,10 +4988,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5000,7 +5049,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
+        <v>501</v>
+      </c>
       <c r="B7" s="5" t="s">
         <v>139</v>
       </c>
@@ -5017,7 +5069,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>500</v>
+      </c>
       <c r="B8" s="5" t="s">
         <v>140</v>
       </c>
@@ -5034,7 +5089,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="50" t="s">
+        <v>499</v>
+      </c>
       <c r="B9" s="5" t="s">
         <v>141</v>
       </c>
@@ -5245,6 +5303,11 @@
         <v>256</v>
       </c>
     </row>
+    <row r="28" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="D28" s="66" t="s">
+        <v>495</v>
+      </c>
+    </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>488</v>
@@ -5278,6 +5341,11 @@
     <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>494</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>498</v>
       </c>
     </row>
   </sheetData>
@@ -5291,7 +5359,7 @@
   <dimension ref="A2:O30"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5606,9 +5674,12 @@
         <v>397</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B27" s="11" t="s">
         <v>253</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -5619,6 +5690,9 @@
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="22" t="s">
         <v>255</v>
+      </c>
+      <c r="D29" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -5636,8 +5710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6575,7 +6649,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
H- Solved all Confilicts Coming from The Dev Team
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="503">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1969,6 +1969,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1983,9 +1986,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2274,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2302,6 +2302,9 @@
       <c r="F2" s="32" t="s">
         <v>185</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
@@ -3029,6 +3032,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3051,30 +3055,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="J1" s="63" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="J1" s="64" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="O1" s="64" t="s">
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="O1" s="65" t="s">
         <v>313</v>
       </c>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="T1" s="65" t="s">
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="T1" s="66" t="s">
         <v>314</v>
       </c>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
@@ -3854,16 +3858,16 @@
       <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F2" s="13" t="s">
@@ -4431,7 +4435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -5304,7 +5308,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="61" t="s">
         <v>495</v>
       </c>
     </row>

</xml_diff>

<commit_message>
H- Fixed The Whole Dependency Issues , SSIS is fully running again , modified lots of ETL Mapps in The Identity Logic
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="505">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1555,6 +1555,12 @@
   </si>
   <si>
     <t>Columns : [CustomerAmount], [MerchantAmount] Needs to be revisited by meeting with Zain &amp; khalaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if type=='OUT' then 1 else  4 </t>
+  </si>
+  <si>
+    <t>handled_by(fetched from the Identity)</t>
   </si>
 </sst>
 </file>
@@ -2274,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3834,8 +3840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4392,7 +4398,7 @@
       <c r="C23" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="56" t="s">
         <v>497</v>
       </c>
     </row>
@@ -4436,7 +4442,7 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4994,8 +5000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5188,8 +5194,8 @@
       <c r="C14" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>143</v>
+      <c r="D14" s="54" t="s">
+        <v>504</v>
       </c>
       <c r="F14" t="s">
         <v>105</v>
@@ -5362,8 +5368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5601,6 +5607,9 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
         <v>418</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>503</v>
       </c>
       <c r="G18" t="s">
         <v>405</v>

</xml_diff>

<commit_message>
H- Modified The REF_Banks and added the vw_ref_banks_final and the whole Workflow is valid up till the Orders & Orders Meta
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="827"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="505">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1211,9 +1211,6 @@
     <t>2-Src Table of Currency</t>
   </si>
   <si>
-    <t>3-Src Table of PWGTypes</t>
-  </si>
-  <si>
     <t>4-Src Table of ChannelTypes</t>
   </si>
   <si>
@@ -1461,9 +1458,6 @@
   </si>
   <si>
     <t>char</t>
-  </si>
-  <si>
-    <t>fk_Customers</t>
   </si>
   <si>
     <t>convert(char(6),first_six)+'******'+convert(char(4),last_four)</t>
@@ -1561,6 +1555,12 @@
   </si>
   <si>
     <t>handled_by(fetched from the Identity)</t>
+  </si>
+  <si>
+    <t>3-Src Table of PGWTypes</t>
+  </si>
+  <si>
+    <t>fk_Customers([old_Customer_Id]=merchant_card_holder_id)</t>
   </si>
 </sst>
 </file>
@@ -2280,20 +2280,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
         <v>391</v>
       </c>
@@ -2309,10 +2309,10 @@
         <v>185</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>188</v>
       </c>
@@ -2322,7 +2322,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2334,7 +2334,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="15" t="s">
         <v>187</v>
@@ -2348,7 +2348,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="15" t="s">
         <v>155</v>
@@ -2362,7 +2362,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="15" t="s">
         <v>156</v>
@@ -2376,7 +2376,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="15"/>
       <c r="C8" s="10"/>
@@ -2388,7 +2388,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="15"/>
       <c r="C9" s="10"/>
@@ -2400,8 +2400,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>392</v>
       </c>
@@ -2417,10 +2417,10 @@
         <v>185</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>274</v>
       </c>
@@ -2430,7 +2430,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="15"/>
       <c r="C13" s="10"/>
@@ -2442,7 +2442,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="15" t="s">
         <v>273</v>
@@ -2456,10 +2456,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
-        <v>393</v>
+        <v>503</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>186</v>
@@ -2472,8 +2472,11 @@
       <c r="F16" s="32" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H16" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>279</v>
       </c>
@@ -2483,7 +2486,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="15"/>
       <c r="C18" s="10"/>
@@ -2495,7 +2498,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="15" t="s">
         <v>273</v>
@@ -2509,10 +2512,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>186</v>
@@ -2525,8 +2528,11 @@
       <c r="F21" s="32" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H21" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>281</v>
       </c>
@@ -2536,7 +2542,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2548,7 +2554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
         <v>282</v>
@@ -2562,7 +2568,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2574,7 +2580,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -2586,7 +2592,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2598,7 +2604,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2610,10 +2616,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B30" s="32" t="s">
         <v>186</v>
@@ -2626,8 +2632,11 @@
       <c r="F30" s="32" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H30" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>285</v>
       </c>
@@ -2637,7 +2646,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -2649,7 +2658,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>286</v>
@@ -2663,7 +2672,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -2675,7 +2684,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2687,7 +2696,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -2699,7 +2708,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -2711,7 +2720,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -2723,10 +2732,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B40" s="32" t="s">
         <v>186</v>
@@ -2740,10 +2749,10 @@
         <v>185</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>296</v>
       </c>
@@ -2753,7 +2762,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -2765,7 +2774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
         <v>297</v>
@@ -2779,7 +2788,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -2791,7 +2800,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -2803,7 +2812,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -2815,7 +2824,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2827,7 +2836,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -2839,29 +2848,29 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="32" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B50" s="32" t="s">
         <v>186</v>
       </c>
       <c r="C50" s="32"/>
       <c r="D50" s="32" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="32" t="s">
         <v>185</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -2869,7 +2878,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -2881,7 +2890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
         <v>141</v>
@@ -2895,7 +2904,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -2907,7 +2916,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -2917,7 +2926,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -2927,7 +2936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -2937,14 +2946,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F58" s="56" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="32" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B59" s="32" t="s">
         <v>186</v>
@@ -2958,7 +2967,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>303</v>
       </c>
@@ -2968,7 +2977,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -2980,7 +2989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="10" t="s">
         <v>221</v>
@@ -2994,7 +3003,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -3006,7 +3015,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -3016,7 +3025,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -3026,7 +3035,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -3046,21 +3055,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E1" s="63" t="s">
         <v>311</v>
       </c>
@@ -3086,7 +3095,7 @@
       <c r="V1" s="66"/>
       <c r="W1" s="66"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>309</v>
       </c>
@@ -3112,7 +3121,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>111</v>
       </c>
@@ -3135,7 +3144,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H4" s="44" t="s">
         <v>364</v>
       </c>
@@ -3149,7 +3158,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>271</v>
       </c>
@@ -3169,7 +3178,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>271</v>
       </c>
@@ -3189,7 +3198,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>271</v>
       </c>
@@ -3209,7 +3218,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>271</v>
       </c>
@@ -3229,7 +3238,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>271</v>
       </c>
@@ -3249,7 +3258,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>271</v>
       </c>
@@ -3266,7 +3275,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>271</v>
       </c>
@@ -3283,7 +3292,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>271</v>
       </c>
@@ -3300,7 +3309,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>271</v>
       </c>
@@ -3317,7 +3326,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>271</v>
       </c>
@@ -3334,7 +3343,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>271</v>
       </c>
@@ -3351,7 +3360,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>271</v>
       </c>
@@ -3368,7 +3377,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>271</v>
       </c>
@@ -3385,7 +3394,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>271</v>
       </c>
@@ -3402,7 +3411,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>271</v>
       </c>
@@ -3419,7 +3428,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>271</v>
       </c>
@@ -3436,7 +3445,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>271</v>
       </c>
@@ -3453,7 +3462,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>271</v>
       </c>
@@ -3470,7 +3479,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>271</v>
       </c>
@@ -3487,7 +3496,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>271</v>
       </c>
@@ -3504,7 +3513,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>271</v>
       </c>
@@ -3521,7 +3530,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>271</v>
       </c>
@@ -3532,7 +3541,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>271</v>
       </c>
@@ -3543,7 +3552,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>271</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>271</v>
       </c>
@@ -3565,7 +3574,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>271</v>
       </c>
@@ -3576,7 +3585,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>271</v>
       </c>
@@ -3587,7 +3596,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>271</v>
       </c>
@@ -3598,7 +3607,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>271</v>
       </c>
@@ -3609,7 +3618,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>271</v>
       </c>
@@ -3620,7 +3629,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>271</v>
       </c>
@@ -3631,7 +3640,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>271</v>
       </c>
@@ -3645,7 +3654,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>271</v>
       </c>
@@ -3656,7 +3665,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>271</v>
       </c>
@@ -3667,7 +3676,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>271</v>
       </c>
@@ -3678,7 +3687,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>271</v>
       </c>
@@ -3689,7 +3698,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>271</v>
       </c>
@@ -3700,7 +3709,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>271</v>
       </c>
@@ -3711,7 +3720,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>271</v>
       </c>
@@ -3722,7 +3731,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>290</v>
       </c>
@@ -3733,7 +3742,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>301</v>
       </c>
@@ -3741,42 +3750,42 @@
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="30" t="s">
         <v>256</v>
       </c>
@@ -3798,37 +3807,37 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -3840,24 +3849,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>135</v>
       </c>
@@ -3875,7 +3884,7 @@
       <c r="M1" s="62"/>
       <c r="N1" s="62"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F2" s="13" t="s">
         <v>181</v>
       </c>
@@ -3895,7 +3904,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>158</v>
       </c>
@@ -3906,7 +3915,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>161</v>
       </c>
@@ -3935,7 +3944,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>161</v>
       </c>
@@ -3964,7 +3973,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>161</v>
       </c>
@@ -3990,7 +3999,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>161</v>
       </c>
@@ -4016,7 +4025,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>161</v>
       </c>
@@ -4045,7 +4054,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>161</v>
       </c>
@@ -4071,7 +4080,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>161</v>
       </c>
@@ -4100,7 +4109,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>161</v>
       </c>
@@ -4129,7 +4138,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>161</v>
       </c>
@@ -4149,7 +4158,7 @@
         <v>119</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>119</v>
@@ -4158,7 +4167,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>161</v>
       </c>
@@ -4187,7 +4196,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>161</v>
       </c>
@@ -4216,7 +4225,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>161</v>
       </c>
@@ -4245,7 +4254,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F16" s="14" t="s">
         <v>157</v>
       </c>
@@ -4265,7 +4274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>158</v>
       </c>
@@ -4291,7 +4300,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>183</v>
       </c>
@@ -4314,7 +4323,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>183</v>
       </c>
@@ -4337,7 +4346,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>183</v>
       </c>
@@ -4348,22 +4357,22 @@
         <v>168</v>
       </c>
       <c r="G20" s="58" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I20" s="58" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K20" s="58" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="N20" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>183</v>
       </c>
@@ -4374,7 +4383,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>183</v>
       </c>
@@ -4385,10 +4394,10 @@
         <v>153</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>183</v>
       </c>
@@ -4399,10 +4408,10 @@
         <v>153</v>
       </c>
       <c r="M23" s="56" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>183</v>
       </c>
@@ -4413,19 +4422,19 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
   </sheetData>
@@ -4442,19 +4451,19 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>207</v>
       </c>
@@ -4474,7 +4483,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>208</v>
       </c>
@@ -4485,13 +4494,13 @@
         <v>149</v>
       </c>
       <c r="H4" s="57" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>208</v>
       </c>
@@ -4508,7 +4517,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>208</v>
       </c>
@@ -4525,7 +4534,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>208</v>
       </c>
@@ -4542,7 +4551,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>208</v>
       </c>
@@ -4562,7 +4571,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>208</v>
       </c>
@@ -4579,7 +4588,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>208</v>
       </c>
@@ -4596,7 +4605,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>208</v>
       </c>
@@ -4613,7 +4622,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>208</v>
       </c>
@@ -4630,7 +4639,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>208</v>
       </c>
@@ -4647,7 +4656,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>208</v>
       </c>
@@ -4661,30 +4670,30 @@
         <v>162</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="30" t="s">
         <v>256</v>
       </c>
@@ -4700,21 +4709,21 @@
   <dimension ref="A3:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>207</v>
       </c>
@@ -4738,74 +4747,74 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C5" t="s">
         <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
       </c>
-      <c r="E6" t="s">
-        <v>477</v>
+      <c r="E6" s="28" t="s">
+        <v>504</v>
       </c>
       <c r="G6" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C7" t="s">
         <v>150</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C8" t="s">
         <v>163</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G8" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
         <v>233</v>
       </c>
@@ -4813,43 +4822,43 @@
         <v>150</v>
       </c>
       <c r="E9" s="52" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G9" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="52" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
       </c>
       <c r="E10" s="52" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G10" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C11" t="s">
         <v>150</v>
       </c>
       <c r="E11" s="52" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G11" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
@@ -4858,29 +4867,29 @@
         <v>233</v>
       </c>
       <c r="G12" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="52" t="s">
+        <v>469</v>
+      </c>
+      <c r="C13" t="s">
+        <v>475</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>473</v>
+      </c>
+      <c r="G13" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="52" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="52" t="s">
         <v>470</v>
       </c>
-      <c r="C13" t="s">
-        <v>476</v>
-      </c>
-      <c r="E13" s="52" t="s">
-        <v>474</v>
-      </c>
-      <c r="G13" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="52" t="s">
-        <v>471</v>
-      </c>
       <c r="C14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E14" s="52" t="s">
         <v>155</v>
@@ -4889,12 +4898,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>471</v>
+      </c>
+      <c r="C15" t="s">
         <v>472</v>
-      </c>
-      <c r="C15" t="s">
-        <v>473</v>
       </c>
       <c r="E15" s="52" t="s">
         <v>156</v>
@@ -4903,21 +4912,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="52" t="s">
+        <v>473</v>
+      </c>
+      <c r="C16" t="s">
         <v>474</v>
       </c>
-      <c r="C16" t="s">
-        <v>475</v>
-      </c>
       <c r="E16" s="52" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="52" t="s">
         <v>155</v>
       </c>
@@ -4931,7 +4940,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="52" t="s">
         <v>156</v>
       </c>
@@ -4939,54 +4948,54 @@
         <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="52" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C19" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20" s="56" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G21" s="56" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="30" t="s">
         <v>256</v>
       </c>
@@ -5000,27 +5009,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="172.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="172.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>136</v>
       </c>
@@ -5040,12 +5049,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>138</v>
       </c>
@@ -5059,9 +5068,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>139</v>
@@ -5079,9 +5088,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>140</v>
@@ -5099,9 +5108,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>141</v>
@@ -5119,7 +5128,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>142</v>
       </c>
@@ -5136,7 +5145,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>143</v>
       </c>
@@ -5153,7 +5162,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>144</v>
       </c>
@@ -5161,7 +5170,7 @@
         <v>153</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F12" t="s">
         <v>101</v>
@@ -5170,7 +5179,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>145</v>
       </c>
@@ -5187,7 +5196,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>146</v>
       </c>
@@ -5195,7 +5204,7 @@
         <v>154</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F14" t="s">
         <v>105</v>
@@ -5204,7 +5213,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>147</v>
       </c>
@@ -5221,7 +5230,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>155</v>
       </c>
@@ -5238,7 +5247,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>156</v>
       </c>
@@ -5255,9 +5264,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B18" s="51" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>157</v>
@@ -5269,7 +5278,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="D19" s="17" t="s">
         <v>157</v>
       </c>
@@ -5280,82 +5289,82 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D20" s="51" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F20" s="59" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="D28" s="61" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="56" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="56" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D31" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="56" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="56" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D34" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D35" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -5372,48 +5381,48 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.44140625" customWidth="1"/>
-    <col min="3" max="3" width="6.21875" customWidth="1"/>
-    <col min="4" max="4" width="53.21875" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" customWidth="1"/>
     <col min="11" max="11" width="81" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>421</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -5422,40 +5431,40 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>157</v>
       </c>
       <c r="G6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>139</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G7" t="s">
         <v>92</v>
@@ -5464,12 +5473,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>235</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G8" t="s">
         <v>78</v>
@@ -5478,37 +5487,37 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>236</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>139</v>
       </c>
       <c r="G10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>235</v>
@@ -5520,12 +5529,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
@@ -5534,26 +5543,26 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G14" t="s">
         <v>84</v>
@@ -5562,9 +5571,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -5576,49 +5585,49 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H16" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>142</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>246</v>
       </c>
@@ -5632,7 +5641,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>155</v>
       </c>
@@ -5646,12 +5655,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>156</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G21" t="s">
         <v>50</v>
@@ -5660,9 +5669,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D22" s="53" t="s">
         <v>157</v>
@@ -5674,41 +5683,41 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" s="22" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G23" s="60" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
         <v>253</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
         <v>255</v>
       </c>
       <c r="D29" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="30" t="s">
         <v>256</v>
       </c>
@@ -5723,26 +5732,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>111</v>
       </c>
@@ -5759,11 +5768,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>271</v>
       </c>
@@ -5783,7 +5792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>271</v>
       </c>
@@ -5803,7 +5812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>271</v>
       </c>
@@ -5823,7 +5832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>271</v>
       </c>
@@ -5843,7 +5852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>271</v>
       </c>
@@ -5863,7 +5872,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>271</v>
       </c>
@@ -5883,7 +5892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>271</v>
       </c>
@@ -5903,7 +5912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>271</v>
       </c>
@@ -5923,7 +5932,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>271</v>
       </c>
@@ -5943,7 +5952,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>271</v>
       </c>
@@ -5963,7 +5972,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>271</v>
       </c>
@@ -5983,7 +5992,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>271</v>
       </c>
@@ -6003,7 +6012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>271</v>
       </c>
@@ -6023,7 +6032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>271</v>
       </c>
@@ -6043,7 +6052,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>271</v>
       </c>
@@ -6063,7 +6072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>271</v>
       </c>
@@ -6083,7 +6092,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>271</v>
       </c>
@@ -6103,7 +6112,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>271</v>
       </c>
@@ -6123,7 +6132,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>271</v>
       </c>
@@ -6143,7 +6152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>271</v>
       </c>
@@ -6163,7 +6172,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>271</v>
       </c>
@@ -6183,7 +6192,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>271</v>
       </c>
@@ -6203,7 +6212,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>271</v>
       </c>
@@ -6223,7 +6232,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>271</v>
       </c>
@@ -6243,7 +6252,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>271</v>
       </c>
@@ -6263,7 +6272,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>271</v>
       </c>
@@ -6274,7 +6283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>271</v>
       </c>
@@ -6282,7 +6291,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>271</v>
       </c>
@@ -6299,7 +6308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>271</v>
       </c>
@@ -6319,7 +6328,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>271</v>
       </c>
@@ -6339,7 +6348,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>271</v>
       </c>
@@ -6359,7 +6368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>271</v>
       </c>
@@ -6379,7 +6388,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>271</v>
       </c>
@@ -6399,7 +6408,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>271</v>
       </c>
@@ -6419,7 +6428,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>271</v>
       </c>
@@ -6439,7 +6448,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>271</v>
       </c>
@@ -6459,7 +6468,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>271</v>
       </c>
@@ -6467,7 +6476,7 @@
         <v>175</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E41" t="s">
         <v>266</v>
@@ -6479,7 +6488,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>271</v>
       </c>
@@ -6487,7 +6496,7 @@
         <v>176</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E42" t="s">
         <v>266</v>
@@ -6499,7 +6508,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>271</v>
       </c>
@@ -6516,7 +6525,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>290</v>
       </c>
@@ -6536,7 +6545,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>301</v>
       </c>
@@ -6556,7 +6565,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D46" s="36" t="s">
         <v>174</v>
       </c>
@@ -6570,7 +6579,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>305</v>
       </c>
@@ -6587,7 +6596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>306</v>
       </c>
@@ -6604,7 +6613,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D49" s="35" t="s">
         <v>157</v>
       </c>
@@ -6618,35 +6627,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D50" s="36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="30" t="s">
         <v>256</v>
       </c>
@@ -6661,40 +6670,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>54</v>
@@ -6703,17 +6712,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>436</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>409</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>437</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -6722,40 +6731,40 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D9" s="53" t="s">
         <v>157</v>
       </c>
       <c r="F9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>139</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F10" t="s">
         <v>92</v>
@@ -6764,12 +6773,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>235</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F11" t="s">
         <v>78</v>
@@ -6778,37 +6787,37 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>236</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F12" t="s">
+        <v>432</v>
+      </c>
+      <c r="G12" t="s">
         <v>433</v>
       </c>
-      <c r="G12" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>139</v>
       </c>
       <c r="F13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>235</v>
@@ -6820,12 +6829,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F15" t="s">
         <v>28</v>
@@ -6834,21 +6843,21 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D16" s="55"/>
       <c r="F16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D17" s="55"/>
       <c r="F17" t="s">
@@ -6858,9 +6867,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -6872,52 +6881,52 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D19" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F19" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>142</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F20" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D21" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F21" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G21" t="s">
         <v>90</v>
       </c>
       <c r="H21" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>246</v>
       </c>
@@ -6931,7 +6940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
         <v>155</v>
       </c>
@@ -6945,12 +6954,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
         <v>156</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F24" t="s">
         <v>50</v>
@@ -6959,9 +6968,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D25" s="53" t="s">
         <v>157</v>
@@ -6973,30 +6982,30 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D26" s="22" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F29" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>253</v>
       </c>
@@ -7004,26 +7013,26 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>254</v>
       </c>
       <c r="D31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="30" t="s">
         <v>256</v>
       </c>

</xml_diff>

<commit_message>
H- Added the Order Transactions Initially  !
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="534">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1640,12 +1640,21 @@
   <si>
     <t>FK_TransactionStatusType</t>
   </si>
+  <si>
+    <t>we are only transferring transactions when model is 'App\Models\Order' and  'App\Modules\Order\Models\Order'</t>
+  </si>
+  <si>
+    <t>[PGWMetaRequest] Needs to be revisited</t>
+  </si>
+  <si>
+    <t>[PGWMetaResponse] Needs to be Revisited</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1807,6 +1816,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1927,7 +1942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2031,9 +2046,6 @@
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2070,6 +2082,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2478,7 +2496,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="32" t="s">
         <v>392</v>
@@ -2534,7 +2552,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="32" t="s">
         <v>501</v>
@@ -2590,7 +2608,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="32" t="s">
         <v>393</v>
@@ -2694,7 +2712,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="32" t="s">
         <v>394</v>
@@ -2810,7 +2828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="32" t="s">
         <v>395</v>
@@ -2926,7 +2944,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A50" s="32" t="s">
         <v>449</v>
@@ -3024,8 +3042,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="56" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F58" s="56" t="s">
+    <row r="58" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="55" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3148,30 +3166,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="62" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="J1" s="64" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="J1" s="63" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="O1" s="65" t="s">
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="O1" s="64" t="s">
         <v>313</v>
       </c>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="T1" s="66" t="s">
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="T1" s="65" t="s">
         <v>314</v>
       </c>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
@@ -3951,16 +3969,16 @@
       <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F2" s="13" t="s">
@@ -4434,16 +4452,16 @@
       <c r="C20" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="G20" s="58" t="s">
+      <c r="G20" s="57" t="s">
         <v>479</v>
       </c>
-      <c r="I20" s="58" t="s">
+      <c r="I20" s="57" t="s">
         <v>483</v>
       </c>
       <c r="J20" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="K20" s="58" t="s">
+      <c r="K20" s="57" t="s">
         <v>480</v>
       </c>
       <c r="N20" t="s">
@@ -4485,7 +4503,7 @@
       <c r="C23" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="M23" s="56" t="s">
+      <c r="M23" s="55" t="s">
         <v>493</v>
       </c>
     </row>
@@ -4571,7 +4589,7 @@
       <c r="D4" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="57" t="s">
+      <c r="H4" s="56" t="s">
         <v>477</v>
       </c>
       <c r="J4" t="s">
@@ -4885,7 +4903,7 @@
       <c r="C8" t="s">
         <v>163</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="51" t="s">
         <v>464</v>
       </c>
       <c r="G8" t="s">
@@ -4893,13 +4911,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>233</v>
       </c>
       <c r="C9" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="51" t="s">
         <v>465</v>
       </c>
       <c r="G9" t="s">
@@ -4907,13 +4925,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>464</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="51" t="s">
         <v>468</v>
       </c>
       <c r="G10" t="s">
@@ -4921,13 +4939,13 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="51" t="s">
         <v>465</v>
       </c>
       <c r="C11" t="s">
         <v>150</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="51" t="s">
         <v>467</v>
       </c>
       <c r="G11" t="s">
@@ -4941,7 +4959,7 @@
       <c r="C12" t="s">
         <v>150</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="51" t="s">
         <v>233</v>
       </c>
       <c r="G12" t="s">
@@ -4949,13 +4967,13 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="51" t="s">
         <v>467</v>
       </c>
       <c r="C13" t="s">
         <v>473</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="51" t="s">
         <v>471</v>
       </c>
       <c r="G13" t="s">
@@ -4963,13 +4981,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="51" t="s">
         <v>468</v>
       </c>
       <c r="C14" t="s">
         <v>473</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="51" t="s">
         <v>155</v>
       </c>
       <c r="G14" t="s">
@@ -4983,7 +5001,7 @@
       <c r="C15" t="s">
         <v>470</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="51" t="s">
         <v>156</v>
       </c>
       <c r="G15" t="s">
@@ -4991,13 +5009,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="51" t="s">
         <v>471</v>
       </c>
       <c r="C16" t="s">
         <v>472</v>
       </c>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="51" t="s">
         <v>418</v>
       </c>
       <c r="G16" t="s">
@@ -5005,7 +5023,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="51" t="s">
         <v>155</v>
       </c>
       <c r="C17" t="s">
@@ -5019,7 +5037,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="51" t="s">
         <v>156</v>
       </c>
       <c r="C18" t="s">
@@ -5033,7 +5051,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="51" t="s">
         <v>418</v>
       </c>
       <c r="C19" t="s">
@@ -5041,7 +5059,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="56" t="s">
+      <c r="G20" s="55" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5049,7 +5067,7 @@
       <c r="E21" t="s">
         <v>412</v>
       </c>
-      <c r="G21" s="56" t="s">
+      <c r="G21" s="55" t="s">
         <v>412</v>
       </c>
     </row>
@@ -5087,8 +5105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5147,7 +5165,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="49" t="s">
         <v>497</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -5156,7 +5174,7 @@
       <c r="C7" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>191</v>
       </c>
       <c r="F7" t="s">
@@ -5176,7 +5194,7 @@
       <c r="C8" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="53" t="s">
         <v>190</v>
       </c>
       <c r="F8" t="s">
@@ -5187,7 +5205,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="49" t="s">
         <v>495</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -5281,7 +5299,7 @@
       <c r="C14" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="53" t="s">
         <v>500</v>
       </c>
       <c r="F14" t="s">
@@ -5343,7 +5361,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>408</v>
       </c>
       <c r="D18" s="17" t="s">
@@ -5368,10 +5386,10 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="50" t="s">
         <v>408</v>
       </c>
-      <c r="F20" s="59" t="s">
+      <c r="F20" s="58" t="s">
         <v>425</v>
       </c>
     </row>
@@ -5401,7 +5419,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="D28" s="61" t="s">
+      <c r="D28" s="60" t="s">
         <v>491</v>
       </c>
     </row>
@@ -5411,7 +5429,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="55" t="s">
         <v>485</v>
       </c>
     </row>
@@ -5426,7 +5444,7 @@
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="56" t="s">
+      <c r="D33" s="55" t="s">
         <v>488</v>
       </c>
     </row>
@@ -5455,8 +5473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5491,7 +5509,7 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="49" t="s">
         <v>444</v>
       </c>
     </row>
@@ -5527,7 +5545,7 @@
       <c r="B6" t="s">
         <v>410</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="52" t="s">
         <v>157</v>
       </c>
       <c r="G6" t="s">
@@ -5751,7 +5769,7 @@
       <c r="B22" s="22" t="s">
         <v>418</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="D22" s="52" t="s">
         <v>157</v>
       </c>
       <c r="G22" t="s">
@@ -5765,7 +5783,7 @@
       <c r="D23" s="22" t="s">
         <v>415</v>
       </c>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="59" t="s">
         <v>443</v>
       </c>
     </row>
@@ -5811,7 +5829,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6433,7 +6451,7 @@
       <c r="B35" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="66" t="s">
         <v>385</v>
       </c>
       <c r="E35" t="s">
@@ -6453,7 +6471,7 @@
       <c r="B36" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D36" s="49" t="s">
+      <c r="D36" s="67" t="s">
         <v>386</v>
       </c>
       <c r="E36" t="s">
@@ -6755,17 +6773,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="77.33203125" bestFit="1" customWidth="1"/>
@@ -6800,12 +6818,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="49" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="51" t="s">
         <v>408</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -6961,7 +6979,7 @@
       <c r="B16" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="D16" s="55" t="s">
+      <c r="D16" s="54" t="s">
         <v>125</v>
       </c>
       <c r="F16" t="s">
@@ -6978,7 +6996,7 @@
       <c r="B17" t="s">
         <v>414</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="54" t="s">
         <v>125</v>
       </c>
       <c r="F17" t="s">
@@ -7117,7 +7135,7 @@
       <c r="B25" s="22" t="s">
         <v>418</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="52" t="s">
         <v>157</v>
       </c>
       <c r="F25" t="s">
@@ -7183,36 +7201,50 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="51" t="s">
         <v>408</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B36" s="28" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D36" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="30" t="s">
         <v>256</v>
+      </c>
+      <c r="D40" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H-Added the Order Transaction_Jsons
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Orders-Meta" sheetId="1" r:id="rId8"/>
     <sheet name="OrderTransactions" sheetId="3" r:id="rId9"/>
     <sheet name="Transactions_Jsons" sheetId="7" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="547">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -971,217 +972,13 @@
     <t>BOSTA</t>
   </si>
   <si>
-    <t>VALU</t>
-  </si>
-  <si>
-    <t>DIXI</t>
-  </si>
-  <si>
-    <t>{"paymentExpiry":"1631138500000"}</t>
-  </si>
-  <si>
     <t>paymentExpiry</t>
   </si>
   <si>
     <t>{</t>
   </si>
   <si>
-    <t xml:space="preserve">  "Address": "asdasd",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Apartment": 123123,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "Floor": 123123,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "CityCode": "asdasdsa",</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  "District": "asdasd"</t>
-  </si>
-  <si>
     <t>}</t>
-  </si>
-  <si>
-    <t>  "isTokenized": false,</t>
-  </si>
-  <si>
-    <t>  "cardNumber": "411111******1111",</t>
-  </si>
-  <si>
-    <t>  "cardExpMonth": "01",</t>
-  </si>
-  <si>
-    <t>  "cardExpYear": "2024",</t>
-  </si>
-  <si>
-    <t>  "cardCvv": "000",</t>
-  </si>
-  <si>
-    <t>  "customerFirstName": "John",</t>
-  </si>
-  <si>
-    <t>  "customerLastName": "Doe",</t>
-  </si>
-  <si>
-    <t>  "customerAddress": "Big Street",</t>
-  </si>
-  <si>
-    <t>  "customerCountry": "US",</t>
-  </si>
-  <si>
-    <t>  "customerState": "CA",</t>
-  </si>
-  <si>
-    <t>  "customerCity": "City",</t>
-  </si>
-  <si>
-    <t>  "customerZip": "123456",</t>
-  </si>
-  <si>
-    <t>  "customerIP": "123.123.123.123",</t>
-  </si>
-  <si>
-    <t>  "rReturnUrl3DS": "http://client.site.com/return.php",</t>
-  </si>
-  <si>
-    <t>  "isRecurring": true,</t>
-  </si>
-  <si>
-    <t>  "cardToken": null,</t>
-  </si>
-  <si>
-    <t>  "gatewayTargetMethod": 1,</t>
-  </si>
-  <si>
-    <t>  "merchantReferenceId": "445579199",</t>
-  </si>
-  <si>
-    <t>  "customerMerchantProfileId": "11111",</t>
-  </si>
-  <si>
-    <t>  "merchantId": 209,</t>
-  </si>
-  <si>
-    <t>  "merchantCode": "78d00363-2b44-4f67-a778-4c016f14f6ed",</t>
-  </si>
-  <si>
-    <t>  "amount": 110,</t>
-  </si>
-  <si>
-    <t>  "description": "Product",</t>
-  </si>
-  <si>
-    <t>  "paymentGatewayTypeId": 0,</t>
-  </si>
-  <si>
-    <t>  "channelType": 0,</t>
-  </si>
-  <si>
-    <t>  "customerName": "ahmed",</t>
-  </si>
-  <si>
-    <t>  "customerMobile": "01008606003",</t>
-  </si>
-  <si>
-    <t>  "customerEmail": "doe@example.com",</t>
-  </si>
-  <si>
-    <t>  "returnURL": null,</t>
-  </si>
-  <si>
-    <t>  "isFeesOnCustomer": true,</t>
-  </si>
-  <si>
-    <t>  "paymentLinkTypeId": 0,</t>
-  </si>
-  <si>
-    <t>  "paymentLinkId": null,</t>
-  </si>
-  <si>
-    <t>  "commession": {</t>
-  </si>
-  <si>
-    <t>    "payMethodType": 1,</t>
-  </si>
-  <si>
-    <t>    "fixedVal": 10,</t>
-  </si>
-  <si>
-    <t>    "percentage": 10,</t>
-  </si>
-  <si>
-    <t>    "isEnabled": true</t>
-  </si>
-  <si>
-    <t>  },</t>
-  </si>
-  <si>
-    <t>  "PromoCode": null,</t>
-  </si>
-  <si>
-    <t>  "ExtraData": null</t>
-  </si>
-  <si>
-    <t>  "_id": null,</t>
-  </si>
-  <si>
-    <t>  "trackingNumber": null,</t>
-  </si>
-  <si>
-    <t>  "message": null,</t>
-  </si>
-  <si>
-    <t>  "Response": null,</t>
-  </si>
-  <si>
-    <t>  "recurringToken": null,</t>
-  </si>
-  <si>
-    <t>  "result": "SUCCESS",</t>
-  </si>
-  <si>
-    <t>  "status": "SETTLED",</t>
-  </si>
-  <si>
-    <t>  "order_id": "560",</t>
-  </si>
-  <si>
-    <t>  "trans_id": "36245-26950-27251",</t>
-  </si>
-  <si>
-    <t>  "trans_date": "2022-09-06 08:24:55",</t>
-  </si>
-  <si>
-    <t>  "descriptor": "test",</t>
-  </si>
-  <si>
-    <t>  "recurring_token": "2d97251945708e420f1c983ce63bed17",</t>
-  </si>
-  <si>
-    <t>  "amount": null,</t>
-  </si>
-  <si>
-    <t>  "card_token": null,</t>
-  </si>
-  <si>
-    <t>  "error_message": null,</t>
-  </si>
-  <si>
-    <t>  "action": "SALE",</t>
-  </si>
-  <si>
-    <t>  "currency": null,</t>
-  </si>
-  <si>
-    <t>  "card_number": "4111111111111111",</t>
-  </si>
-  <si>
-    <t>  "card_exp_month": "01",</t>
-  </si>
-  <si>
-    <t>  "card_exp_year": "2024"</t>
   </si>
   <si>
     <t>mostly all jsons are from Merchants</t>
@@ -1649,12 +1446,255 @@
   <si>
     <t>[PGWMetaResponse] Needs to be Revisited</t>
   </si>
+  <si>
+    <t xml:space="preserve">  "action": "Sale",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "cardNumber": "411111******1111",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "cardExpMonth": "01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "cardExpYear": "2024",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "isTokenized": true,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "isRecurring": true,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "customerEmail": "doe@example.com",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "period": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "initPeriod": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "times": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "cardToken": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "termUrl3ds": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "transId": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "recurringToken": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "recurringFirstTransId": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "amount": 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "recurringToken": "a8487693d860e33126901437ebe63c4c",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "transId": "36438-11578-47321",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "cardToken": "94317d84b0483e31b43210925138c5186377a6be5d029057ee70ecddac9f47dd",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "transDate": "2022-09-28 16:05:57",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "redirectUrl": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "redirectParams": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "redirectMethod": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "status": "SETTLED",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "descriptor": "test",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "authCode": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "declineReason": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "creditvoidDate": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "amount": null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "address": "ssdaaaassdasd",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "apartment": 2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "floor": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "cityCode": "EG-01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "district": "ddd"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "customerEmail": "ahmed@gmail.com",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "referenceNumber": "7105039001"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "paymentExpiry": "1631138500000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "VendorName": "InitPay jmeter",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "MobileNumber": "01029981337",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "ProductId": "EGMHOC23DP4",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "OrderId": "Refrencejmeter3430Va1",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "DownPayment": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "ToUAmount": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "CashbackAmount": 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "loanNumber": "CL091022517636",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "transactionId": "091022222705048"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "tahweelQR": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "mVisaQR": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "validity": "jhjh",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "consumerMobileNumber": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "loyaltyNumber": "asasN",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "customerLabel": "CL",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "purposeOfTransaction": "Test",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "billNumber": "01001920550",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "convenienceFeeFixed": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "convenienceFeePercentage": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "dateTimeLocalTrxn": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "tip": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "gatewayTargetMethod": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "merchantReferenceId": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "customerMerchantProfileId": "11111",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "merchantId": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "merchantCode": "00000000-0000-0000-0000-000000000000",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "amount": 10,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "description": "string",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "paymentGatewayTypeId": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "channelType": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "customerFirstName": "ahmed",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "customerLastName": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "customerMobile": "01008606003",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "returnURL": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "isFeesOnCustomer": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "paymentLinkTypeId": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "paymentLinkId": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "commession": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "PromoCode": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "ExtraData": null</t>
+  </si>
+  <si>
+    <t>VALU (Msh M3ana)</t>
+  </si>
+  <si>
+    <t>DIXI (Akurateko)</t>
+  </si>
+  <si>
+    <t>UPG(Meeza)</t>
+  </si>
+  <si>
+    <t>merchant_callback_url</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1744,13 +1784,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color rgb="FFDCDCDC"/>
       <name val="Consolas"/>
@@ -1821,6 +1854,30 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1942,7 +1999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2035,21 +2092,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
@@ -2061,12 +2115,18 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2083,12 +2143,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2391,7 +2455,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="32" t="s">
-        <v>391</v>
+        <v>323</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>186</v>
@@ -2405,7 +2469,7 @@
         <v>185</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>481</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
@@ -2496,10 +2560,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="32" t="s">
-        <v>392</v>
+        <v>324</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>186</v>
@@ -2513,7 +2577,7 @@
         <v>185</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>481</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
@@ -2552,10 +2616,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="32" t="s">
-        <v>501</v>
+        <v>433</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>186</v>
@@ -2569,7 +2633,7 @@
         <v>185</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>481</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2608,10 +2672,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="32" t="s">
-        <v>393</v>
+        <v>325</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>186</v>
@@ -2625,7 +2689,7 @@
         <v>185</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>481</v>
+        <v>413</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2712,10 +2776,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="32" t="s">
-        <v>394</v>
+        <v>326</v>
       </c>
       <c r="B30" s="32" t="s">
         <v>186</v>
@@ -2729,7 +2793,7 @@
         <v>185</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>481</v>
+        <v>413</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2828,10 +2892,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="32" t="s">
-        <v>395</v>
+        <v>327</v>
       </c>
       <c r="B40" s="32" t="s">
         <v>186</v>
@@ -2845,7 +2909,7 @@
         <v>185</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>481</v>
+        <v>413</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2944,29 +3008,29 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A50" s="32" t="s">
-        <v>449</v>
+        <v>381</v>
       </c>
       <c r="B50" s="32" t="s">
         <v>186</v>
       </c>
       <c r="C50" s="32"/>
       <c r="D50" s="32" t="s">
-        <v>450</v>
+        <v>382</v>
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="32" t="s">
         <v>185</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>481</v>
+        <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
-        <v>451</v>
+        <v>383</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -3042,14 +3106,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F58" s="55" t="s">
+    <row r="58" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F58" s="54" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A59" s="32" t="s">
-        <v>452</v>
+        <v>384</v>
       </c>
       <c r="B59" s="32" t="s">
         <v>186</v>
@@ -3149,10 +3213,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W61"/>
+  <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:W1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3160,38 +3224,50 @@
     <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
+    <col min="18" max="18" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="83.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="E1" s="62" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="E1" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="J1" s="63" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="J1" s="64" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="O1" s="64" t="s">
-        <v>313</v>
-      </c>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="T1" s="65" t="s">
-        <v>314</v>
-      </c>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="O1" s="65" t="s">
+        <v>543</v>
+      </c>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="T1" s="66" t="s">
+        <v>544</v>
+      </c>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="Z1" s="62" t="s">
+        <v>545</v>
+      </c>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
         <v>309</v>
       </c>
@@ -3216,527 +3292,632 @@
       <c r="W2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="Z2" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="41" t="s">
-        <v>315</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>317</v>
-      </c>
-      <c r="M3" s="47" t="s">
-        <v>317</v>
-      </c>
-      <c r="P3" s="43" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="H4" s="44" t="s">
-        <v>364</v>
-      </c>
-      <c r="K4" s="46" t="s">
-        <v>318</v>
-      </c>
-      <c r="M4" s="47" t="s">
-        <v>364</v>
-      </c>
-      <c r="P4" s="43" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="F3" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>314</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>314</v>
+      </c>
+      <c r="M3" s="69"/>
+      <c r="P3" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="R3" s="70" t="s">
+        <v>314</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB3" s="72"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="F4" s="68" t="s">
+        <v>502</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>501</v>
+      </c>
+      <c r="K4" s="45" t="s">
+        <v>495</v>
+      </c>
+      <c r="M4" s="46"/>
+      <c r="P4" s="42" t="s">
+        <v>503</v>
+      </c>
+      <c r="R4" s="71" t="s">
+        <v>510</v>
+      </c>
+      <c r="U4" t="s">
+        <v>466</v>
+      </c>
+      <c r="W4" t="s">
+        <v>482</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="H5" s="44" t="s">
-        <v>365</v>
-      </c>
-      <c r="K5" s="46" t="s">
-        <v>319</v>
-      </c>
-      <c r="M5" s="47" t="s">
-        <v>365</v>
-      </c>
-      <c r="P5" s="43" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="F5" s="68" t="s">
+        <v>315</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>315</v>
+      </c>
+      <c r="K5" s="45" t="s">
+        <v>496</v>
+      </c>
+      <c r="M5" s="46"/>
+      <c r="P5" s="42" t="s">
+        <v>504</v>
+      </c>
+      <c r="R5" s="71" t="s">
+        <v>511</v>
+      </c>
+      <c r="U5" t="s">
+        <v>467</v>
+      </c>
+      <c r="W5" t="s">
+        <v>483</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="H6" s="44" t="s">
-        <v>366</v>
-      </c>
-      <c r="K6" s="46" t="s">
-        <v>320</v>
-      </c>
-      <c r="M6" s="47" t="s">
-        <v>366</v>
-      </c>
-      <c r="P6" s="43" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H6" s="43"/>
+      <c r="K6" s="45" t="s">
+        <v>497</v>
+      </c>
+      <c r="M6" s="46"/>
+      <c r="P6" s="42" t="s">
+        <v>505</v>
+      </c>
+      <c r="R6" s="71" t="s">
+        <v>315</v>
+      </c>
+      <c r="U6" t="s">
+        <v>468</v>
+      </c>
+      <c r="W6" t="s">
+        <v>484</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="H7" s="44" t="s">
-        <v>367</v>
-      </c>
-      <c r="K7" s="46" t="s">
-        <v>321</v>
-      </c>
-      <c r="M7" s="47" t="s">
-        <v>367</v>
-      </c>
-      <c r="P7" s="43" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H7" s="43"/>
+      <c r="K7" s="45" t="s">
+        <v>498</v>
+      </c>
+      <c r="M7" s="46"/>
+      <c r="P7" s="42" t="s">
+        <v>506</v>
+      </c>
+      <c r="U7" t="s">
+        <v>469</v>
+      </c>
+      <c r="W7" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>368</v>
-      </c>
-      <c r="K8" s="46" t="s">
-        <v>322</v>
-      </c>
-      <c r="M8" s="47" t="s">
-        <v>368</v>
-      </c>
-      <c r="P8" s="43" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H8" s="43"/>
+      <c r="K8" s="45" t="s">
+        <v>499</v>
+      </c>
+      <c r="M8" s="46"/>
+      <c r="P8" s="42" t="s">
+        <v>507</v>
+      </c>
+      <c r="U8" t="s">
+        <v>470</v>
+      </c>
+      <c r="W8" t="s">
+        <v>486</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="H9" s="44" t="s">
-        <v>339</v>
-      </c>
-      <c r="K9" s="46" t="s">
-        <v>323</v>
-      </c>
-      <c r="M9" s="47" t="s">
-        <v>339</v>
-      </c>
-      <c r="P9" s="43" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H9" s="43"/>
+      <c r="K9" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="M9" s="46"/>
+      <c r="P9" s="42" t="s">
+        <v>508</v>
+      </c>
+      <c r="U9" t="s">
+        <v>471</v>
+      </c>
+      <c r="W9" t="s">
+        <v>487</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="H10" s="44" t="s">
-        <v>369</v>
-      </c>
-      <c r="M10" s="47" t="s">
-        <v>369</v>
-      </c>
-      <c r="P10" s="43" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H10" s="43"/>
+      <c r="M10" s="46"/>
+      <c r="P10" s="42" t="s">
+        <v>509</v>
+      </c>
+      <c r="U10" t="s">
+        <v>472</v>
+      </c>
+      <c r="W10" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="H11" s="44" t="s">
-        <v>370</v>
-      </c>
-      <c r="M11" s="47" t="s">
-        <v>370</v>
-      </c>
-      <c r="P11" s="43" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H11" s="43"/>
+      <c r="M11" s="46"/>
+      <c r="P11" s="42" t="s">
+        <v>315</v>
+      </c>
+      <c r="U11" t="s">
+        <v>473</v>
+      </c>
+      <c r="W11" t="s">
+        <v>489</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="H12" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="M12" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="P12" s="43" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H12" s="43"/>
+      <c r="M12" s="46"/>
+      <c r="P12" s="42"/>
+      <c r="U12" t="s">
+        <v>474</v>
+      </c>
+      <c r="W12" t="s">
+        <v>490</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="H13" s="44" t="s">
-        <v>372</v>
-      </c>
-      <c r="M13" s="47" t="s">
-        <v>372</v>
-      </c>
-      <c r="P13" s="43" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H13" s="43"/>
+      <c r="M13" s="46"/>
+      <c r="P13" s="42"/>
+      <c r="U13" t="s">
+        <v>475</v>
+      </c>
+      <c r="W13" t="s">
+        <v>491</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="H14" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="M14" s="47" t="s">
-        <v>373</v>
-      </c>
-      <c r="P14" s="43" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H14" s="43"/>
+      <c r="M14" s="46"/>
+      <c r="P14" s="42"/>
+      <c r="U14" t="s">
+        <v>476</v>
+      </c>
+      <c r="W14" t="s">
+        <v>492</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="H15" s="44" t="s">
-        <v>374</v>
-      </c>
-      <c r="M15" s="47" t="s">
-        <v>374</v>
-      </c>
-      <c r="P15" s="43" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H15" s="43"/>
+      <c r="M15" s="46"/>
+      <c r="P15" s="42"/>
+      <c r="U15" t="s">
+        <v>477</v>
+      </c>
+      <c r="W15" t="s">
+        <v>493</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="H16" s="44" t="s">
-        <v>375</v>
-      </c>
-      <c r="M16" s="47" t="s">
-        <v>375</v>
-      </c>
-      <c r="P16" s="43" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H16" s="43"/>
+      <c r="M16" s="46"/>
+      <c r="P16" s="42"/>
+      <c r="U16" t="s">
+        <v>478</v>
+      </c>
+      <c r="W16" t="s">
+        <v>494</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="H17" s="44" t="s">
-        <v>376</v>
-      </c>
-      <c r="M17" s="47" t="s">
-        <v>376</v>
-      </c>
-      <c r="P17" s="43" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H17" s="43"/>
+      <c r="M17" s="46"/>
+      <c r="P17" s="42"/>
+      <c r="U17" t="s">
+        <v>479</v>
+      </c>
+      <c r="W17" t="s">
+        <v>315</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="H18" s="44" t="s">
-        <v>377</v>
-      </c>
-      <c r="M18" s="47" t="s">
-        <v>377</v>
-      </c>
-      <c r="P18" s="43" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H18" s="43"/>
+      <c r="M18" s="46"/>
+      <c r="P18" s="42"/>
+      <c r="U18" t="s">
+        <v>480</v>
+      </c>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="11" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>229</v>
       </c>
-      <c r="H19" s="44" t="s">
-        <v>378</v>
-      </c>
-      <c r="M19" s="47" t="s">
-        <v>378</v>
-      </c>
-      <c r="P19" s="43" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H19" s="43"/>
+      <c r="M19" s="46"/>
+      <c r="P19" s="42"/>
+      <c r="U19" t="s">
+        <v>481</v>
+      </c>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="11" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="H20" s="44" t="s">
-        <v>379</v>
-      </c>
-      <c r="M20" s="47" t="s">
-        <v>379</v>
-      </c>
-      <c r="P20" s="43" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H20" s="43"/>
+      <c r="M20" s="46"/>
+      <c r="P20" s="42"/>
+      <c r="U20" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="11" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="H21" s="44" t="s">
-        <v>380</v>
-      </c>
-      <c r="M21" s="47" t="s">
-        <v>380</v>
-      </c>
-      <c r="P21" s="43" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H21" s="43"/>
+      <c r="M21" s="46"/>
+      <c r="P21" s="42"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="11" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="H22" s="44" t="s">
-        <v>381</v>
-      </c>
-      <c r="M22" s="47" t="s">
-        <v>381</v>
-      </c>
-      <c r="P22" s="43" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H22" s="43"/>
+      <c r="M22" s="46"/>
+      <c r="P22" s="42"/>
+      <c r="Y22" s="51"/>
+      <c r="Z22" s="11" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="H23" s="44" t="s">
-        <v>382</v>
-      </c>
-      <c r="M23" s="47" t="s">
-        <v>382</v>
-      </c>
-      <c r="P23" s="43" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H23" s="43"/>
+      <c r="M23" s="46"/>
+      <c r="P23" s="42"/>
+      <c r="Z23" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="H24" s="44" t="s">
-        <v>383</v>
-      </c>
-      <c r="M24" s="47" t="s">
-        <v>383</v>
-      </c>
-      <c r="P24" s="43" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H24" s="43"/>
+      <c r="M24" s="46"/>
+      <c r="P24" s="42"/>
+      <c r="Y24" s="51"/>
+      <c r="Z24" s="11" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="H25" s="44" t="s">
-        <v>323</v>
-      </c>
-      <c r="M25" s="47" t="s">
-        <v>323</v>
-      </c>
-      <c r="P25" s="43" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="H25" s="43"/>
+      <c r="M25" s="46"/>
+      <c r="P25" s="42"/>
+      <c r="Y25" s="51"/>
+      <c r="Z25" s="11" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B26" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="P26" s="43" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P26" s="42"/>
+      <c r="Z26" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="P27" s="43" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P27" s="42"/>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="11" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B28" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="P28" s="43" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P28" s="42"/>
+      <c r="Y28" s="51"/>
+      <c r="Z28" s="11" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="P29" s="43" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P29" s="42"/>
+      <c r="Y29" s="51" t="s">
+        <v>546</v>
+      </c>
+      <c r="Z29" s="11" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B30" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="P30" s="43" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P30" s="42"/>
+      <c r="Z30" s="11" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="P31" s="43" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P31" s="42"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="P32" s="43" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P32" s="42"/>
+      <c r="Y32" s="51"/>
+      <c r="Z32" s="11" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B33" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="P33" s="43" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P33" s="42"/>
+      <c r="Y33" s="51"/>
+      <c r="Z33" s="11" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>241</v>
       </c>
-      <c r="P34" s="43" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P34" s="42"/>
+      <c r="Y34" s="51"/>
+      <c r="Z34" s="11" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="P35" s="43" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P35" s="42"/>
+      <c r="Z35" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>271</v>
       </c>
@@ -3744,101 +3925,88 @@
         <v>243</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="P36" s="48" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+      <c r="P36" s="47"/>
+      <c r="Z36" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B37" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="P37" s="43" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P37" s="42"/>
+    </row>
+    <row r="38" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B38" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="P38" s="43" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P38" s="42"/>
+    </row>
+    <row r="39" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="P39" s="43" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P39" s="42"/>
+    </row>
+    <row r="40" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="P40" s="43" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P40" s="42"/>
+    </row>
+    <row r="41" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="P41" s="43" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P41" s="42"/>
+    </row>
+    <row r="42" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="P42" s="43" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P42" s="42"/>
+    </row>
+    <row r="43" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" s="31" t="s">
         <v>271</v>
       </c>
       <c r="B43" t="s">
         <v>247</v>
       </c>
-      <c r="P43" s="43" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P43" s="42"/>
+    </row>
+    <row r="44" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
         <v>290</v>
       </c>
       <c r="B44" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="P44" s="42" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="P44" s="41" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" s="31" t="s">
         <v>301</v>
       </c>
@@ -3846,17 +4014,17 @@
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>306</v>
       </c>
@@ -3887,14 +4055,27 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="T1:W1"/>
+    <mergeCell ref="Z1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3913,27 +4094,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>387</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>389</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>390</v>
+        <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>427</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3969,16 +4150,16 @@
       <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F2" s="13" t="s">
@@ -4254,7 +4435,7 @@
         <v>119</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>482</v>
+        <v>414</v>
       </c>
       <c r="K12" s="11" t="s">
         <v>119</v>
@@ -4452,20 +4633,20 @@
       <c r="C20" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="G20" s="57" t="s">
-        <v>479</v>
-      </c>
-      <c r="I20" s="57" t="s">
-        <v>483</v>
+      <c r="G20" s="56" t="s">
+        <v>411</v>
+      </c>
+      <c r="I20" s="56" t="s">
+        <v>415</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>408</v>
-      </c>
-      <c r="K20" s="57" t="s">
-        <v>480</v>
+        <v>340</v>
+      </c>
+      <c r="K20" s="56" t="s">
+        <v>412</v>
       </c>
       <c r="N20" t="s">
-        <v>442</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -4490,7 +4671,7 @@
         <v>153</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>492</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -4503,8 +4684,8 @@
       <c r="C23" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="M23" s="55" t="s">
-        <v>493</v>
+      <c r="M23" s="54" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="18" x14ac:dyDescent="0.35">
@@ -4589,8 +4770,8 @@
       <c r="D4" t="s">
         <v>149</v>
       </c>
-      <c r="H4" s="56" t="s">
-        <v>477</v>
+      <c r="H4" s="55" t="s">
+        <v>409</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
@@ -4766,12 +4947,12 @@
         <v>162</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>478</v>
+        <v>410</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="28" t="s">
-        <v>396</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.3">
@@ -4845,10 +5026,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>460</v>
+        <v>392</v>
       </c>
       <c r="B4" t="s">
-        <v>408</v>
+        <v>340</v>
       </c>
       <c r="C4" t="s">
         <v>163</v>
@@ -4856,13 +5037,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>412</v>
+        <v>344</v>
       </c>
       <c r="C5" t="s">
         <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>436</v>
+        <v>368</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -4870,27 +5051,27 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>461</v>
+        <v>393</v>
       </c>
       <c r="C6" t="s">
         <v>150</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>502</v>
+        <v>434</v>
       </c>
       <c r="G6" t="s">
-        <v>453</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>462</v>
+        <v>394</v>
       </c>
       <c r="C7" t="s">
         <v>150</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>474</v>
+        <v>406</v>
       </c>
       <c r="G7" t="s">
         <v>260</v>
@@ -4898,96 +5079,96 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>463</v>
+        <v>395</v>
       </c>
       <c r="C8" t="s">
         <v>163</v>
       </c>
-      <c r="E8" s="51" t="s">
-        <v>464</v>
+      <c r="E8" s="50" t="s">
+        <v>396</v>
       </c>
       <c r="G8" t="s">
-        <v>454</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="50" t="s">
         <v>233</v>
       </c>
       <c r="C9" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="51" t="s">
-        <v>465</v>
+      <c r="E9" s="50" t="s">
+        <v>397</v>
       </c>
       <c r="G9" t="s">
-        <v>455</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="51" t="s">
-        <v>464</v>
+      <c r="B10" s="50" t="s">
+        <v>396</v>
       </c>
       <c r="C10" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="51" t="s">
-        <v>468</v>
+      <c r="E10" s="50" t="s">
+        <v>400</v>
       </c>
       <c r="G10" t="s">
-        <v>456</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="51" t="s">
-        <v>465</v>
+      <c r="B11" s="50" t="s">
+        <v>397</v>
       </c>
       <c r="C11" t="s">
         <v>150</v>
       </c>
-      <c r="E11" s="51" t="s">
-        <v>467</v>
+      <c r="E11" s="50" t="s">
+        <v>399</v>
       </c>
       <c r="G11" t="s">
-        <v>457</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>466</v>
+        <v>398</v>
       </c>
       <c r="C12" t="s">
         <v>150</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="50" t="s">
         <v>233</v>
       </c>
       <c r="G12" t="s">
-        <v>458</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="51" t="s">
-        <v>467</v>
+      <c r="B13" s="50" t="s">
+        <v>399</v>
       </c>
       <c r="C13" t="s">
-        <v>473</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>471</v>
+        <v>405</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>403</v>
       </c>
       <c r="G13" t="s">
-        <v>459</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="51" t="s">
-        <v>468</v>
+      <c r="B14" s="50" t="s">
+        <v>400</v>
       </c>
       <c r="C14" t="s">
-        <v>473</v>
-      </c>
-      <c r="E14" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="E14" s="50" t="s">
         <v>155</v>
       </c>
       <c r="G14" t="s">
@@ -4996,12 +5177,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>469</v>
+        <v>401</v>
       </c>
       <c r="C15" t="s">
-        <v>470</v>
-      </c>
-      <c r="E15" s="51" t="s">
+        <v>402</v>
+      </c>
+      <c r="E15" s="50" t="s">
         <v>156</v>
       </c>
       <c r="G15" t="s">
@@ -5009,21 +5190,21 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="51" t="s">
-        <v>471</v>
+      <c r="B16" s="50" t="s">
+        <v>403</v>
       </c>
       <c r="C16" t="s">
-        <v>472</v>
-      </c>
-      <c r="E16" s="51" t="s">
-        <v>418</v>
+        <v>404</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>350</v>
       </c>
       <c r="G16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="50" t="s">
         <v>155</v>
       </c>
       <c r="C17" t="s">
@@ -5037,43 +5218,43 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>156</v>
       </c>
       <c r="C18" t="s">
         <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>461</v>
+        <v>393</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>476</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="51" t="s">
-        <v>418</v>
+      <c r="B19" s="50" t="s">
+        <v>350</v>
       </c>
       <c r="C19" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="55" t="s">
-        <v>475</v>
+      <c r="G20" s="54" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>412</v>
-      </c>
-      <c r="G21" s="55" t="s">
-        <v>412</v>
+        <v>344</v>
+      </c>
+      <c r="G21" s="54" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22" s="28" t="s">
-        <v>396</v>
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -5147,7 +5328,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>445</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5165,8 +5346,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49" t="s">
-        <v>497</v>
+      <c r="A7" s="48" t="s">
+        <v>429</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>139</v>
@@ -5174,7 +5355,7 @@
       <c r="C7" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="52" t="s">
         <v>191</v>
       </c>
       <c r="F7" t="s">
@@ -5186,7 +5367,7 @@
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>496</v>
+        <v>428</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>140</v>
@@ -5194,7 +5375,7 @@
       <c r="C8" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="52" t="s">
         <v>190</v>
       </c>
       <c r="F8" t="s">
@@ -5205,8 +5386,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
-        <v>495</v>
+      <c r="A9" s="48" t="s">
+        <v>427</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>141</v>
@@ -5266,7 +5447,7 @@
         <v>153</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>446</v>
+        <v>378</v>
       </c>
       <c r="F12" t="s">
         <v>101</v>
@@ -5299,8 +5480,8 @@
       <c r="C14" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="53" t="s">
-        <v>500</v>
+      <c r="D14" s="52" t="s">
+        <v>432</v>
       </c>
       <c r="F14" t="s">
         <v>105</v>
@@ -5361,8 +5542,8 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B18" s="50" t="s">
-        <v>408</v>
+      <c r="B18" s="49" t="s">
+        <v>340</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>157</v>
@@ -5386,16 +5567,16 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="50" t="s">
-        <v>408</v>
-      </c>
-      <c r="F20" s="58" t="s">
-        <v>425</v>
+      <c r="D20" s="49" t="s">
+        <v>340</v>
+      </c>
+      <c r="F20" s="57" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="28" t="s">
-        <v>396</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -5419,48 +5600,48 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="D28" s="60" t="s">
-        <v>491</v>
+      <c r="D28" s="59" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>484</v>
+        <v>416</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="55" t="s">
-        <v>485</v>
+      <c r="D30" s="54" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>486</v>
+        <v>418</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>487</v>
+        <v>419</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="55" t="s">
-        <v>488</v>
+      <c r="D33" s="54" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>489</v>
+        <v>421</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>490</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>494</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -5492,16 +5673,16 @@
   <sheetData>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>407</v>
+        <v>339</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>419</v>
+        <v>351</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>420</v>
+        <v>352</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>406</v>
+        <v>338</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>56</v>
@@ -5509,16 +5690,16 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
-        <v>444</v>
+      <c r="A3" s="48" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>408</v>
+        <v>340</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>421</v>
+        <v>353</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -5529,13 +5710,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>409</v>
+        <v>341</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>422</v>
+        <v>354</v>
       </c>
       <c r="G5" t="s">
-        <v>397</v>
+        <v>329</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -5543,13 +5724,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>410</v>
-      </c>
-      <c r="D6" s="52" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6" s="51" t="s">
         <v>157</v>
       </c>
       <c r="G6" t="s">
-        <v>398</v>
+        <v>330</v>
       </c>
       <c r="H6" t="s">
         <v>76</v>
@@ -5560,7 +5741,7 @@
         <v>139</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>430</v>
+        <v>362</v>
       </c>
       <c r="G7" t="s">
         <v>92</v>
@@ -5574,7 +5755,7 @@
         <v>235</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="G8" t="s">
         <v>78</v>
@@ -5588,24 +5769,24 @@
         <v>236</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>424</v>
+        <v>356</v>
       </c>
       <c r="G9" t="s">
-        <v>399</v>
+        <v>331</v>
       </c>
       <c r="H9" t="s">
-        <v>405</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>411</v>
+        <v>343</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>139</v>
       </c>
       <c r="G10" t="s">
-        <v>400</v>
+        <v>332</v>
       </c>
       <c r="H10" t="s">
         <v>81</v>
@@ -5613,7 +5794,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>412</v>
+        <v>344</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>235</v>
@@ -5627,10 +5808,10 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>413</v>
+        <v>345</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>426</v>
+        <v>358</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
@@ -5641,13 +5822,13 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>423</v>
+        <v>355</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>429</v>
+        <v>361</v>
       </c>
       <c r="G13" t="s">
-        <v>401</v>
+        <v>333</v>
       </c>
       <c r="H13" t="s">
         <v>31</v>
@@ -5655,10 +5836,10 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>414</v>
+        <v>346</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>429</v>
+        <v>361</v>
       </c>
       <c r="G14" t="s">
         <v>84</v>
@@ -5669,7 +5850,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>415</v>
+        <v>347</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -5683,13 +5864,13 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>416</v>
+        <v>348</v>
       </c>
       <c r="D16" t="s">
-        <v>428</v>
+        <v>360</v>
       </c>
       <c r="G16" t="s">
-        <v>402</v>
+        <v>334</v>
       </c>
       <c r="H16" t="s">
         <v>88</v>
@@ -5700,10 +5881,10 @@
         <v>142</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>417</v>
+        <v>349</v>
       </c>
       <c r="G17" t="s">
-        <v>403</v>
+        <v>335</v>
       </c>
       <c r="H17" t="s">
         <v>89</v>
@@ -5711,13 +5892,13 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
-        <v>417</v>
+        <v>349</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>499</v>
+        <v>431</v>
       </c>
       <c r="G18" t="s">
-        <v>404</v>
+        <v>336</v>
       </c>
       <c r="H18" t="s">
         <v>90</v>
@@ -5756,7 +5937,7 @@
         <v>156</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>418</v>
+        <v>350</v>
       </c>
       <c r="G21" t="s">
         <v>50</v>
@@ -5767,9 +5948,9 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="D22" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="D22" s="51" t="s">
         <v>157</v>
       </c>
       <c r="G22" t="s">
@@ -5781,15 +5962,15 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D23" s="22" t="s">
-        <v>415</v>
-      </c>
-      <c r="G23" s="59" t="s">
-        <v>443</v>
+        <v>347</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="28" t="s">
-        <v>396</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
@@ -5797,7 +5978,7 @@
         <v>253</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>492</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -5810,7 +5991,7 @@
         <v>255</v>
       </c>
       <c r="D29" t="s">
-        <v>498</v>
+        <v>430</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -5829,7 +6010,7 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6451,8 +6632,8 @@
       <c r="B35" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="D35" s="66" t="s">
-        <v>385</v>
+      <c r="D35" s="60" t="s">
+        <v>317</v>
       </c>
       <c r="E35" t="s">
         <v>266</v>
@@ -6471,8 +6652,8 @@
       <c r="B36" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D36" s="67" t="s">
-        <v>386</v>
+      <c r="D36" s="61" t="s">
+        <v>318</v>
       </c>
       <c r="E36" t="s">
         <v>266</v>
@@ -6572,7 +6753,7 @@
         <v>175</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>441</v>
+        <v>373</v>
       </c>
       <c r="E41" t="s">
         <v>266</v>
@@ -6592,7 +6773,7 @@
         <v>176</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>441</v>
+        <v>373</v>
       </c>
       <c r="E42" t="s">
         <v>266</v>
@@ -6725,18 +6906,18 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D50" s="36" t="s">
-        <v>408</v>
+        <v>340</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>442</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B57" s="28" t="s">
-        <v>396</v>
+        <v>328</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>492</v>
+        <v>424</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.3">
@@ -6749,7 +6930,7 @@
         <v>254</v>
       </c>
       <c r="D59" t="s">
-        <v>503</v>
+        <v>435</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.3">
@@ -6757,7 +6938,7 @@
         <v>255</v>
       </c>
       <c r="D60" t="s">
-        <v>504</v>
+        <v>436</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.3">
@@ -6775,7 +6956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -6802,13 +6983,13 @@
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>407</v>
+        <v>339</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>434</v>
+        <v>366</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>420</v>
+        <v>352</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>54</v>
@@ -6818,16 +6999,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49" t="s">
-        <v>435</v>
+      <c r="A6" s="48" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="51" t="s">
-        <v>408</v>
+      <c r="B7" s="50" t="s">
+        <v>340</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>436</v>
+        <v>368</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -6841,36 +7022,36 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>409</v>
+        <v>341</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>436</v>
+        <v>368</v>
       </c>
       <c r="F8" t="s">
-        <v>397</v>
+        <v>329</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>506</v>
+        <v>438</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>410</v>
+        <v>342</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>423</v>
+        <v>355</v>
       </c>
       <c r="F9" t="s">
-        <v>398</v>
+        <v>330</v>
       </c>
       <c r="G9" t="s">
         <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>507</v>
+        <v>439</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -6878,7 +7059,7 @@
         <v>139</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>437</v>
+        <v>369</v>
       </c>
       <c r="F10" t="s">
         <v>92</v>
@@ -6887,7 +7068,7 @@
         <v>77</v>
       </c>
       <c r="I10" t="s">
-        <v>508</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -6895,7 +7076,7 @@
         <v>235</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>438</v>
+        <v>370</v>
       </c>
       <c r="F11" t="s">
         <v>78</v>
@@ -6904,7 +7085,7 @@
         <v>79</v>
       </c>
       <c r="I11" t="s">
-        <v>509</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -6912,38 +7093,38 @@
         <v>236</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>505</v>
+        <v>437</v>
       </c>
       <c r="F12" t="s">
-        <v>432</v>
+        <v>364</v>
       </c>
       <c r="G12" t="s">
-        <v>433</v>
+        <v>365</v>
       </c>
       <c r="I12" t="s">
-        <v>510</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>411</v>
+        <v>343</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>139</v>
       </c>
       <c r="F13" t="s">
-        <v>400</v>
+        <v>332</v>
       </c>
       <c r="G13" t="s">
         <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>511</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>412</v>
+        <v>344</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>235</v>
@@ -6955,15 +7136,15 @@
         <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>512</v>
+        <v>444</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>413</v>
+        <v>345</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>426</v>
+        <v>358</v>
       </c>
       <c r="F15" t="s">
         <v>28</v>
@@ -6972,31 +7153,31 @@
         <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>513</v>
+        <v>445</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="D16" s="54" t="s">
+        <v>355</v>
+      </c>
+      <c r="D16" s="53" t="s">
         <v>125</v>
       </c>
       <c r="F16" t="s">
-        <v>401</v>
+        <v>333</v>
       </c>
       <c r="G16" t="s">
         <v>31</v>
       </c>
       <c r="I16" t="s">
-        <v>514</v>
+        <v>446</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>414</v>
-      </c>
-      <c r="D17" s="54" t="s">
+        <v>346</v>
+      </c>
+      <c r="D17" s="53" t="s">
         <v>125</v>
       </c>
       <c r="F17" t="s">
@@ -7006,12 +7187,12 @@
         <v>85</v>
       </c>
       <c r="I17" t="s">
-        <v>515</v>
+        <v>447</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>415</v>
+        <v>347</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -7023,24 +7204,24 @@
         <v>87</v>
       </c>
       <c r="I18" t="s">
-        <v>516</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>416</v>
+        <v>348</v>
       </c>
       <c r="D19" t="s">
-        <v>428</v>
+        <v>360</v>
       </c>
       <c r="F19" t="s">
-        <v>402</v>
+        <v>334</v>
       </c>
       <c r="G19" t="s">
         <v>88</v>
       </c>
       <c r="I19" t="s">
-        <v>517</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
@@ -7048,36 +7229,36 @@
         <v>142</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>417</v>
+        <v>349</v>
       </c>
       <c r="F20" t="s">
-        <v>403</v>
+        <v>335</v>
       </c>
       <c r="G20" t="s">
         <v>89</v>
       </c>
       <c r="I20" t="s">
-        <v>518</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="28" t="s">
-        <v>417</v>
+        <v>349</v>
       </c>
       <c r="D21" t="s">
-        <v>448</v>
+        <v>380</v>
       </c>
       <c r="F21" t="s">
-        <v>404</v>
+        <v>336</v>
       </c>
       <c r="G21" t="s">
         <v>90</v>
       </c>
       <c r="H21" t="s">
-        <v>447</v>
+        <v>379</v>
       </c>
       <c r="I21" t="s">
-        <v>519</v>
+        <v>451</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -7094,7 +7275,7 @@
         <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>520</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
@@ -7111,7 +7292,7 @@
         <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>521</v>
+        <v>453</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
@@ -7119,7 +7300,7 @@
         <v>156</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>418</v>
+        <v>350</v>
       </c>
       <c r="F24" t="s">
         <v>50</v>
@@ -7128,14 +7309,14 @@
         <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>522</v>
+        <v>454</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="22" t="s">
-        <v>418</v>
-      </c>
-      <c r="D25" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="D25" s="51" t="s">
         <v>157</v>
       </c>
       <c r="F25" t="s">
@@ -7145,7 +7326,7 @@
         <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>523</v>
+        <v>455</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
@@ -7153,13 +7334,13 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>529</v>
+        <v>461</v>
       </c>
       <c r="G26" t="s">
-        <v>530</v>
+        <v>462</v>
       </c>
       <c r="I26" t="s">
-        <v>524</v>
+        <v>456</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -7167,7 +7348,7 @@
         <v>263</v>
       </c>
       <c r="I27" t="s">
-        <v>525</v>
+        <v>457</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -7175,7 +7356,7 @@
         <v>68</v>
       </c>
       <c r="I28" t="s">
-        <v>526</v>
+        <v>458</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -7183,10 +7364,10 @@
         <v>125</v>
       </c>
       <c r="F29" t="s">
-        <v>439</v>
+        <v>371</v>
       </c>
       <c r="I29" t="s">
-        <v>527</v>
+        <v>459</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
@@ -7194,26 +7375,26 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>440</v>
+        <v>372</v>
       </c>
       <c r="I30" t="s">
-        <v>528</v>
+        <v>460</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D31" s="51" t="s">
-        <v>408</v>
+      <c r="D31" s="50" t="s">
+        <v>340</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>442</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B36" s="28" t="s">
-        <v>396</v>
+        <v>328</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>492</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
@@ -7221,7 +7402,7 @@
         <v>253</v>
       </c>
       <c r="D37" t="s">
-        <v>531</v>
+        <v>463</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
@@ -7239,12 +7420,12 @@
         <v>256</v>
       </c>
       <c r="D40" t="s">
-        <v>532</v>
+        <v>464</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>533</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H-Modified The Transactions Mapping Sheet
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -2128,6 +2128,16 @@
     <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2143,16 +2153,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3215,8 +3215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="X12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK18" sqref="AK18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3237,35 +3237,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="69" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="J1" s="64" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="J1" s="70" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="O1" s="65" t="s">
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="O1" s="71" t="s">
         <v>543</v>
       </c>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="T1" s="66" t="s">
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="T1" s="72" t="s">
         <v>544</v>
       </c>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="Z1" s="62" t="s">
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
+      <c r="Z1" s="68" t="s">
         <v>545</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="F2" t="s">
@@ -3306,7 +3306,7 @@
       <c r="B3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="67" t="s">
+      <c r="F3" s="62" t="s">
         <v>314</v>
       </c>
       <c r="H3" s="43" t="s">
@@ -3315,11 +3315,11 @@
       <c r="K3" s="44" t="s">
         <v>314</v>
       </c>
-      <c r="M3" s="69"/>
+      <c r="M3" s="64"/>
       <c r="P3" s="42" t="s">
         <v>314</v>
       </c>
-      <c r="R3" s="70" t="s">
+      <c r="R3" s="65" t="s">
         <v>314</v>
       </c>
       <c r="U3" s="3" t="s">
@@ -3331,10 +3331,10 @@
       <c r="Z3" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="AB3" s="72"/>
+      <c r="AB3" s="67"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="63" t="s">
         <v>502</v>
       </c>
       <c r="H4" s="43" t="s">
@@ -3347,7 +3347,7 @@
       <c r="P4" s="42" t="s">
         <v>503</v>
       </c>
-      <c r="R4" s="71" t="s">
+      <c r="R4" s="66" t="s">
         <v>510</v>
       </c>
       <c r="U4" t="s">
@@ -3367,7 +3367,7 @@
       <c r="B5" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="F5" s="63" t="s">
         <v>315</v>
       </c>
       <c r="H5" s="43" t="s">
@@ -3380,7 +3380,7 @@
       <c r="P5" s="42" t="s">
         <v>504</v>
       </c>
-      <c r="R5" s="71" t="s">
+      <c r="R5" s="66" t="s">
         <v>511</v>
       </c>
       <c r="U5" t="s">
@@ -3408,7 +3408,7 @@
       <c r="P6" s="42" t="s">
         <v>505</v>
       </c>
-      <c r="R6" s="71" t="s">
+      <c r="R6" s="66" t="s">
         <v>315</v>
       </c>
       <c r="U6" t="s">
@@ -3754,7 +3754,7 @@
       <c r="H23" s="43"/>
       <c r="M23" s="46"/>
       <c r="P23" s="42"/>
-      <c r="Z23" t="s">
+      <c r="Z23" s="11" t="s">
         <v>531</v>
       </c>
     </row>
@@ -4150,16 +4150,16 @@
       <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="68" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F2" s="13" t="s">
@@ -4728,7 +4728,7 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
H-Added The Transaction Balance Table to Mapping Sheet and Implemented it
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Orders-Meta" sheetId="1" r:id="rId8"/>
     <sheet name="OrderTransactions" sheetId="3" r:id="rId9"/>
     <sheet name="Transactions_Jsons" sheetId="7" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId11"/>
+    <sheet name="Transaction_Balance" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="559">
   <si>
     <t xml:space="preserve">  FROM [TransactionManagement].[dbo].[Orders]</t>
   </si>
@@ -1689,12 +1689,48 @@
   <si>
     <t>merchant_callback_url</t>
   </si>
+  <si>
+    <t>TransactionBalance TRGT Columns</t>
+  </si>
+  <si>
+    <t>Src_Table Transactions_Balance from Staging Area</t>
+  </si>
+  <si>
+    <t>OrderTransactions</t>
+  </si>
+  <si>
+    <t>[Old_Id]</t>
+  </si>
+  <si>
+    <t>[old_WithdrawalTransaction]</t>
+  </si>
+  <si>
+    <t>[TranxId]</t>
+  </si>
+  <si>
+    <t>[TranxTypeId]</t>
+  </si>
+  <si>
+    <t>[ModelTypeId]</t>
+  </si>
+  <si>
+    <t>[ModelReferenceId]</t>
+  </si>
+  <si>
+    <t>[Balance]</t>
+  </si>
+  <si>
+    <t>[AvailableBalance]</t>
+  </si>
+  <si>
+    <t>1 orders, 2 withdrawals</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1879,6 +1915,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -1999,7 +2043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2153,6 +2197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2440,7 +2485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
@@ -4069,13 +4114,309 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="73" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>351</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>549</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>368</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" t="s">
+        <v>329</v>
+      </c>
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C6" t="s">
+        <v>330</v>
+      </c>
+      <c r="E6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" t="s">
+        <v>364</v>
+      </c>
+      <c r="E7" t="s">
+        <v>332</v>
+      </c>
+      <c r="G7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>335</v>
+      </c>
+      <c r="G8" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" t="s">
+        <v>558</v>
+      </c>
+      <c r="G9" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>332</v>
+      </c>
+      <c r="C10" t="s">
+        <v>332</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>250</v>
+      </c>
+      <c r="G11" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G12" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C13" t="s">
+        <v>333</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>371</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>335</v>
+      </c>
+      <c r="C17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>336</v>
+      </c>
+      <c r="C18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>551</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5654,8 +5995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Fixed for 18 Bugs So Far in The Testing
</commit_message>
<xml_diff>
--- a/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
+++ b/All_Migration_Mapping_Sheets/Cowpay_to_Excel_Mapping_Sheet_Transactions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="827" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="827" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hot_LKPs(Banks &amp; Other Lookups)" sheetId="9" r:id="rId1"/>
@@ -2182,6 +2182,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2197,7 +2198,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2489,16 +2489,16 @@
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
         <v>323</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>188</v>
       </c>
@@ -2527,7 +2527,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2539,7 +2539,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="15" t="s">
         <v>187</v>
@@ -2553,7 +2553,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="15" t="s">
         <v>155</v>
@@ -2567,7 +2567,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="15" t="s">
         <v>156</v>
@@ -2581,7 +2581,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="15"/>
       <c r="C8" s="10"/>
@@ -2593,7 +2593,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="15"/>
       <c r="C9" s="10"/>
@@ -2605,8 +2605,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>324</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>274</v>
       </c>
@@ -2635,7 +2635,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="15"/>
       <c r="C13" s="10"/>
@@ -2647,7 +2647,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="15" t="s">
         <v>273</v>
@@ -2661,8 +2661,8 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
         <v>433</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>279</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="15"/>
       <c r="C18" s="10"/>
@@ -2703,7 +2703,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="15" t="s">
         <v>273</v>
@@ -2717,8 +2717,8 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
         <v>325</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>281</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2759,7 +2759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
         <v>282</v>
@@ -2773,7 +2773,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -2785,7 +2785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -2797,7 +2797,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -2809,7 +2809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -2821,8 +2821,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
         <v>326</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>285</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -2863,7 +2863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>286</v>
@@ -2877,7 +2877,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -2889,7 +2889,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2901,7 +2901,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -2913,7 +2913,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -2925,7 +2925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -2937,8 +2937,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="32" t="s">
         <v>327</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>296</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -2979,7 +2979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10" t="s">
         <v>297</v>
@@ -2993,7 +2993,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -3005,7 +3005,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -3017,7 +3017,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -3029,7 +3029,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -3041,7 +3041,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -3053,8 +3053,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="32" t="s">
         <v>381</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>383</v>
       </c>
@@ -3083,7 +3083,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -3095,7 +3095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="10" t="s">
         <v>141</v>
@@ -3109,7 +3109,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -3121,7 +3121,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -3131,7 +3131,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -3141,7 +3141,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -3151,12 +3151,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F58" s="54" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="32" t="s">
         <v>384</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>303</v>
       </c>
@@ -3182,7 +3182,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -3194,7 +3194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="10" t="s">
         <v>221</v>
@@ -3208,7 +3208,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -3220,7 +3220,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -3230,7 +3230,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -3240,7 +3240,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -3264,55 +3264,55 @@
       <selection activeCell="AK18" sqref="AK18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" customWidth="1"/>
-    <col min="18" max="18" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="83.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="83.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="E1" s="69" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="E1" s="70" t="s">
         <v>311</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="J1" s="70" t="s">
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="J1" s="71" t="s">
         <v>312</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="O1" s="71" t="s">
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="O1" s="72" t="s">
         <v>543</v>
       </c>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="T1" s="72" t="s">
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="T1" s="73" t="s">
         <v>544</v>
       </c>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="Z1" s="68" t="s">
+      <c r="U1" s="73"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="Z1" s="69" t="s">
         <v>545</v>
       </c>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
         <v>309</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:28" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>111</v>
       </c>
@@ -3378,7 +3378,7 @@
       </c>
       <c r="AB3" s="67"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="F4" s="63" t="s">
         <v>502</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>271</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>271</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>271</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>271</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>271</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>271</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>271</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>271</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>271</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>271</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>271</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>271</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>271</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>271</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>271</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>271</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>271</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>271</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>271</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>271</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>271</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>271</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>271</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>271</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>271</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>271</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>271</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>271</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>271</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>271</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>271</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>271</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>271</v>
       </c>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="P37" s="42"/>
     </row>
-    <row r="38" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>271</v>
       </c>
@@ -3995,7 +3995,7 @@
       </c>
       <c r="P38" s="42"/>
     </row>
-    <row r="39" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>271</v>
       </c>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="P39" s="42"/>
     </row>
-    <row r="40" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>271</v>
       </c>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="P40" s="42"/>
     </row>
-    <row r="41" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>271</v>
       </c>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="P41" s="42"/>
     </row>
-    <row r="42" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>271</v>
       </c>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="P42" s="42"/>
     </row>
-    <row r="43" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>271</v>
       </c>
@@ -4040,7 +4040,7 @@
       </c>
       <c r="P43" s="42"/>
     </row>
-    <row r="44" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>290</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>301</v>
       </c>
@@ -4059,42 +4059,42 @@
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="28" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="30" t="s">
         <v>256</v>
       </c>
@@ -4116,29 +4116,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="73" t="s">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="68" t="s">
         <v>548</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="68" t="s">
         <v>351</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="68" t="s">
         <v>549</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -4151,7 +4151,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>329</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>330</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>331</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>92</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>78</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>332</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>26</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>333</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>84</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>86</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>334</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>335</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>336</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>48</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>49</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>50</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>55</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>551</v>
       </c>
@@ -4389,27 +4389,27 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>550</v>
       </c>
@@ -4428,32 +4428,32 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>359</v>
       </c>
@@ -4471,38 +4471,38 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.44140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>135</v>
       </c>
       <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="69" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F2" s="13" t="s">
         <v>181</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>158</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>161</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>161</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>161</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>161</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>161</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>161</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>161</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>161</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>161</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>161</v>
       </c>
@@ -4814,7 +4814,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>161</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>161</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F16" s="14" t="s">
         <v>157</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>158</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>183</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>183</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>183</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>183</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>183</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>183</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>183</v>
       </c>
@@ -5040,19 +5040,19 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
   </sheetData>
@@ -5072,16 +5072,16 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>207</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>208</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>208</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>208</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>208</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>208</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>208</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>208</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>208</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>208</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>208</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>208</v>
       </c>
@@ -5291,27 +5291,27 @@
         <v>410</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="28" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="30" t="s">
         <v>256</v>
       </c>
@@ -5330,18 +5330,18 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>207</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>344</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>393</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>394</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>395</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="50" t="s">
         <v>233</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="50" t="s">
         <v>396</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="50" t="s">
         <v>397</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>398</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="50" t="s">
         <v>399</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="50" t="s">
         <v>400</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>401</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="50" t="s">
         <v>403</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="50" t="s">
         <v>155</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="50" t="s">
         <v>156</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="50" t="s">
         <v>350</v>
       </c>
@@ -5580,12 +5580,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G20" s="54" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>344</v>
       </c>
@@ -5593,27 +5593,27 @@
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="28" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="30" t="s">
         <v>256</v>
       </c>
@@ -5631,23 +5631,23 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="172.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="172.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>136</v>
       </c>
@@ -5667,12 +5667,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>138</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>429</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>428</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>427</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>142</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>143</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>144</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>145</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>146</v>
       </c>
@@ -5831,7 +5831,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>147</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
         <v>155</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>156</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B18" s="49" t="s">
         <v>340</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="D19" s="17" t="s">
         <v>157</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D20" s="49" t="s">
         <v>340</v>
       </c>
@@ -5915,72 +5915,72 @@
         <v>357</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="D28" s="59" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D30" s="54" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="54" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>426</v>
       </c>
@@ -5995,24 +5995,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.44140625" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" customWidth="1"/>
-    <col min="8" max="8" width="73.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" customWidth="1"/>
     <col min="11" max="11" width="81" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>339</v>
       </c>
@@ -6030,12 +6030,12 @@
       </c>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>340</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>341</v>
       </c>
@@ -6063,12 +6063,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>342</v>
       </c>
-      <c r="D6" s="51" t="s">
-        <v>157</v>
+      <c r="D6" s="22" t="s">
+        <v>355</v>
       </c>
       <c r="G6" t="s">
         <v>330</v>
@@ -6077,7 +6077,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>139</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
         <v>235</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>236</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>343</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>344</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>345</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
         <v>355</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>346</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>347</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>348</v>
       </c>
@@ -6217,7 +6217,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>142</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="28" t="s">
         <v>349</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>246</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>155</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>156</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
         <v>350</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" s="22" t="s">
         <v>347</v>
       </c>
@@ -6309,12 +6309,12 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="28" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="s">
         <v>253</v>
       </c>
@@ -6322,12 +6322,12 @@
         <v>424</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="22" t="s">
         <v>255</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="30" t="s">
         <v>256</v>
       </c>
@@ -6354,22 +6354,22 @@
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>111</v>
       </c>
@@ -6386,11 +6386,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>271</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>271</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>271</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>271</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>271</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>271</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>271</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>271</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>271</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>271</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>271</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>271</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>271</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>271</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>271</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>271</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>271</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>271</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>271</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>271</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>271</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>271</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>271</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>271</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>271</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>271</v>
       </c>
@@ -6901,7 +6901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>271</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>271</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>271</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>271</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>271</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>271</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>271</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>271</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>271</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>271</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>271</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>271</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>271</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>290</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>301</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D46" s="36" t="s">
         <v>174</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>305</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>306</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D49" s="35" t="s">
         <v>157</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D50" s="36" t="s">
         <v>340</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B57" s="28" t="s">
         <v>328</v>
       </c>
@@ -7261,12 +7261,12 @@
         <v>424</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>254</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="22" t="s">
         <v>255</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="30" t="s">
         <v>256</v>
       </c>
@@ -7301,28 +7301,28 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="98.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="77.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="98.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3"/>
     </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>339</v>
       </c>
@@ -7339,12 +7339,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="50" t="s">
         <v>340</v>
       </c>
@@ -7361,7 +7361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>341</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>342</v>
       </c>
@@ -7395,7 +7395,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>139</v>
       </c>
@@ -7412,7 +7412,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>235</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>236</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>343</v>
       </c>
@@ -7463,7 +7463,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>344</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>345</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
         <v>355</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>346</v>
       </c>
@@ -7531,7 +7531,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>347</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>348</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>142</v>
       </c>
@@ -7582,7 +7582,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
         <v>349</v>
       </c>
@@ -7602,7 +7602,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>246</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
         <v>155</v>
       </c>
@@ -7636,7 +7636,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
         <v>156</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
         <v>350</v>
       </c>
@@ -7670,7 +7670,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>1</v>
       </c>
@@ -7684,7 +7684,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>263</v>
       </c>
@@ -7692,7 +7692,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>68</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>125</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>1</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D31" s="50" t="s">
         <v>340</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B36" s="28" t="s">
         <v>328</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>253</v>
       </c>
@@ -7746,17 +7746,17 @@
         <v>463</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="22" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="30" t="s">
         <v>256</v>
       </c>
@@ -7764,7 +7764,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D41" s="54" t="s">
         <v>465</v>
       </c>

</xml_diff>